<commit_message>
More GUI Bug Fixes
</commit_message>
<xml_diff>
--- a/results/Daily Eff. Report AutoTest.xlsx
+++ b/results/Daily Eff. Report AutoTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabian/Desktop/PythonProject/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6425DFF-4226-3249-A354-BDD996D893B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3184C726-CFB1-E947-A7D5-82BD9CA067BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HILDA 6-MAR" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,9 @@
     <sheet name="RAMON 1-MAY" sheetId="8" r:id="rId8"/>
     <sheet name="SUPERVISOR 1-MAY" sheetId="9" r:id="rId9"/>
     <sheet name="MARCIA 1-MAY" sheetId="10" r:id="rId10"/>
-    <sheet name="ALI 1-MAY1" sheetId="11" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -934,11 +933,13 @@
     <font>
       <sz val="24"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1009,7 +1010,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1652,21 +1653,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1845,6 +1831,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1874,12 +1866,6 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1918,30 +1904,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="44" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2200,7 +2186,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8712-3744-B480-CC3649249E70}"/>
+              <c16:uniqueId val="{00000000-AF21-1A49-85ED-6C1FB20FDD42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2318,7 +2304,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8712-3744-B480-CC3649249E70}"/>
+              <c16:uniqueId val="{00000001-AF21-1A49-85ED-6C1FB20FDD42}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2619,7 +2605,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9D8D-8E4E-960E-508747827832}"/>
+              <c16:uniqueId val="{00000000-2FBA-C348-BD31-2B7311EA5DE6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2740,7 +2726,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9D8D-8E4E-960E-508747827832}"/>
+              <c16:uniqueId val="{00000001-2FBA-C348-BD31-2B7311EA5DE6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3041,7 +3027,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3980-3445-B683-C74A3B78EE5F}"/>
+              <c16:uniqueId val="{00000000-B127-7644-BFC1-2EDFD1F90740}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3162,7 +3148,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3980-3445-B683-C74A3B78EE5F}"/>
+              <c16:uniqueId val="{00000001-B127-7644-BFC1-2EDFD1F90740}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3748,39 +3734,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="56" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="56" customWidth="1"/>
-    <col min="3" max="3" width="74.83203125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="56" customWidth="1"/>
-    <col min="6" max="6" width="31.5" style="56" customWidth="1"/>
-    <col min="7" max="8" width="27.5" style="56" customWidth="1"/>
-    <col min="9" max="9" width="3.5" style="56" customWidth="1"/>
-    <col min="10" max="10" width="37.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" style="58" customWidth="1"/>
-    <col min="15" max="15" width="36.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="45.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.83203125" style="58" customWidth="1"/>
-    <col min="18" max="18" width="13" style="58" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="88.83203125" style="58" customWidth="1"/>
-    <col min="20" max="20" width="27.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="27.5" style="58" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="2.83203125" style="58" customWidth="1"/>
-    <col min="26" max="26" width="39.5" style="58" customWidth="1"/>
-    <col min="30" max="30" width="21.1640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22" style="58" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.33203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="29.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.1640625" style="56" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="20" style="58" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.33203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="29.5" style="56" bestFit="1" customWidth="1"/>
-    <col min="38" max="48" width="8.83203125" style="58" customWidth="1"/>
-    <col min="49" max="130" width="8.83203125" style="56" customWidth="1"/>
-    <col min="131" max="16384" width="8.83203125" style="56"/>
+    <col min="1" max="1" width="25.1640625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="58" customWidth="1"/>
+    <col min="3" max="3" width="74.83203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" style="58" customWidth="1"/>
+    <col min="6" max="6" width="31.5" style="58" customWidth="1"/>
+    <col min="7" max="8" width="27.5" style="58" customWidth="1"/>
+    <col min="9" max="9" width="3.5" style="58" customWidth="1"/>
+    <col min="10" max="10" width="37.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="60" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="60" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.6640625" style="60" customWidth="1"/>
+    <col min="15" max="15" width="36.83203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="45.83203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.83203125" style="60" customWidth="1"/>
+    <col min="18" max="18" width="13" style="60" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="88.83203125" style="60" customWidth="1"/>
+    <col min="20" max="20" width="27.5" style="60" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="27.5" style="60" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="2.83203125" style="60" customWidth="1"/>
+    <col min="26" max="26" width="39.5" style="60" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22" style="60" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.33203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20" style="60" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.33203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="29.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="38" max="48" width="8.83203125" style="60" customWidth="1"/>
+    <col min="49" max="131" width="8.83203125" style="58" customWidth="1"/>
+    <col min="132" max="16384" width="8.83203125" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -3799,28 +3785,28 @@
       <c r="N1" s="3"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="56"/>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AQ1" s="56"/>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="56"/>
-      <c r="AU1" s="56"/>
-      <c r="AV1" s="56"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AL1" s="58"/>
+      <c r="AM1" s="58"/>
+      <c r="AN1" s="58"/>
+      <c r="AO1" s="58"/>
+      <c r="AP1" s="58"/>
+      <c r="AQ1" s="58"/>
+      <c r="AR1" s="58"/>
+      <c r="AS1" s="58"/>
+      <c r="AT1" s="58"/>
+      <c r="AU1" s="58"/>
+      <c r="AV1" s="58"/>
     </row>
     <row r="2" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="82" t="s">
@@ -3838,28 +3824,28 @@
       <c r="N2" s="3"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AE2" s="56"/>
-      <c r="AF2" s="56"/>
-      <c r="AI2" s="56"/>
-      <c r="AJ2" s="56"/>
-      <c r="AL2" s="56"/>
-      <c r="AM2" s="56"/>
-      <c r="AN2" s="56"/>
-      <c r="AO2" s="56"/>
-      <c r="AP2" s="56"/>
-      <c r="AQ2" s="56"/>
-      <c r="AR2" s="56"/>
-      <c r="AS2" s="56"/>
-      <c r="AT2" s="56"/>
-      <c r="AU2" s="56"/>
-      <c r="AV2" s="56"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
     </row>
     <row r="3" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="84" t="s">
@@ -3874,34 +3860,34 @@
       <c r="H3" s="83"/>
       <c r="I3" s="83"/>
       <c r="J3" s="83"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AI3" s="56"/>
-      <c r="AJ3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="56"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="58"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="58"/>
+      <c r="AV3" s="58"/>
     </row>
     <row r="4" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="84" t="s">
@@ -3916,34 +3902,34 @@
       <c r="H4" s="83"/>
       <c r="I4" s="83"/>
       <c r="J4" s="83"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="56"/>
-      <c r="AE4" s="56"/>
-      <c r="AF4" s="56"/>
-      <c r="AI4" s="56"/>
-      <c r="AJ4" s="56"/>
-      <c r="AL4" s="56"/>
-      <c r="AM4" s="56"/>
-      <c r="AN4" s="56"/>
-      <c r="AO4" s="56"/>
-      <c r="AP4" s="56"/>
-      <c r="AQ4" s="56"/>
-      <c r="AR4" s="56"/>
-      <c r="AS4" s="56"/>
-      <c r="AT4" s="56"/>
-      <c r="AU4" s="56"/>
-      <c r="AV4" s="56"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="58"/>
+      <c r="X4" s="58"/>
+      <c r="Y4" s="58"/>
+      <c r="Z4" s="58"/>
+      <c r="AA4" s="58"/>
+      <c r="AB4" s="58"/>
+      <c r="AC4" s="58"/>
+      <c r="AE4" s="58"/>
+      <c r="AF4" s="58"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
+      <c r="AL4" s="58"/>
+      <c r="AM4" s="58"/>
+      <c r="AN4" s="58"/>
+      <c r="AO4" s="58"/>
+      <c r="AP4" s="58"/>
+      <c r="AQ4" s="58"/>
+      <c r="AR4" s="58"/>
+      <c r="AS4" s="58"/>
+      <c r="AT4" s="58"/>
+      <c r="AU4" s="58"/>
+      <c r="AV4" s="58"/>
     </row>
     <row r="5" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="85" t="s">
@@ -3955,10 +3941,10 @@
       <c r="C5" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="59" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -3974,34 +3960,34 @@
       <c r="J5" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="56"/>
-      <c r="Z5" s="56"/>
-      <c r="AA5" s="56"/>
-      <c r="AB5" s="56"/>
-      <c r="AC5" s="56"/>
-      <c r="AE5" s="56"/>
-      <c r="AF5" s="56"/>
-      <c r="AI5" s="56"/>
-      <c r="AJ5" s="56"/>
-      <c r="AL5" s="56"/>
-      <c r="AM5" s="56"/>
-      <c r="AN5" s="56"/>
-      <c r="AO5" s="56"/>
-      <c r="AP5" s="56"/>
-      <c r="AQ5" s="56"/>
-      <c r="AR5" s="56"/>
-      <c r="AS5" s="56"/>
-      <c r="AT5" s="56"/>
-      <c r="AU5" s="56"/>
-      <c r="AV5" s="56"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="58"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58"/>
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="58"/>
+      <c r="AR5" s="58"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
     </row>
     <row r="6" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="86"/>
@@ -4028,34 +4014,34 @@
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="89"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="56"/>
-      <c r="Z6" s="56"/>
-      <c r="AA6" s="56"/>
-      <c r="AB6" s="56"/>
-      <c r="AC6" s="56"/>
-      <c r="AE6" s="56"/>
-      <c r="AF6" s="56"/>
-      <c r="AI6" s="56"/>
-      <c r="AJ6" s="56"/>
-      <c r="AL6" s="56"/>
-      <c r="AM6" s="56"/>
-      <c r="AN6" s="56"/>
-      <c r="AO6" s="56"/>
-      <c r="AP6" s="56"/>
-      <c r="AQ6" s="56"/>
-      <c r="AR6" s="56"/>
-      <c r="AS6" s="56"/>
-      <c r="AT6" s="56"/>
-      <c r="AU6" s="56"/>
-      <c r="AV6" s="56"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+      <c r="AC6" s="58"/>
+      <c r="AE6" s="58"/>
+      <c r="AF6" s="58"/>
+      <c r="AI6" s="58"/>
+      <c r="AJ6" s="58"/>
+      <c r="AL6" s="58"/>
+      <c r="AM6" s="58"/>
+      <c r="AN6" s="58"/>
+      <c r="AO6" s="58"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="58"/>
+      <c r="AR6" s="58"/>
+      <c r="AS6" s="58"/>
+      <c r="AT6" s="58"/>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="58"/>
     </row>
     <row r="7" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="87"/>
@@ -4078,34 +4064,34 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="92"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
-      <c r="Y7" s="56"/>
-      <c r="Z7" s="56"/>
-      <c r="AA7" s="56"/>
-      <c r="AB7" s="56"/>
-      <c r="AC7" s="56"/>
-      <c r="AE7" s="56"/>
-      <c r="AF7" s="56"/>
-      <c r="AI7" s="56"/>
-      <c r="AJ7" s="56"/>
-      <c r="AL7" s="56"/>
-      <c r="AM7" s="56"/>
-      <c r="AN7" s="56"/>
-      <c r="AO7" s="56"/>
-      <c r="AP7" s="56"/>
-      <c r="AQ7" s="56"/>
-      <c r="AR7" s="56"/>
-      <c r="AS7" s="56"/>
-      <c r="AT7" s="56"/>
-      <c r="AU7" s="56"/>
-      <c r="AV7" s="56"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="58"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="58"/>
+      <c r="AL7" s="58"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="58"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="58"/>
+      <c r="AU7" s="58"/>
+      <c r="AV7" s="58"/>
     </row>
     <row r="8" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
@@ -4135,34 +4121,34 @@
         <f t="shared" ref="J8:J13" si="0">AVERAGE(D8:H8)</f>
         <v>42.425000000000004</v>
       </c>
-      <c r="Q8" s="56"/>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="56"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="56"/>
-      <c r="W8" s="56"/>
-      <c r="X8" s="56"/>
-      <c r="Y8" s="56"/>
-      <c r="Z8" s="56"/>
-      <c r="AA8" s="56"/>
-      <c r="AB8" s="56"/>
-      <c r="AC8" s="56"/>
-      <c r="AE8" s="56"/>
-      <c r="AF8" s="56"/>
-      <c r="AI8" s="56"/>
-      <c r="AJ8" s="56"/>
-      <c r="AL8" s="56"/>
-      <c r="AM8" s="56"/>
-      <c r="AN8" s="56"/>
-      <c r="AO8" s="56"/>
-      <c r="AP8" s="56"/>
-      <c r="AQ8" s="56"/>
-      <c r="AR8" s="56"/>
-      <c r="AS8" s="56"/>
-      <c r="AT8" s="56"/>
-      <c r="AU8" s="56"/>
-      <c r="AV8" s="56"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+      <c r="Z8" s="58"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AE8" s="58"/>
+      <c r="AF8" s="58"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AL8" s="58"/>
+      <c r="AM8" s="58"/>
+      <c r="AN8" s="58"/>
+      <c r="AO8" s="58"/>
+      <c r="AP8" s="58"/>
+      <c r="AQ8" s="58"/>
+      <c r="AR8" s="58"/>
+      <c r="AS8" s="58"/>
+      <c r="AT8" s="58"/>
+      <c r="AU8" s="58"/>
+      <c r="AV8" s="58"/>
     </row>
     <row r="9" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
@@ -4192,34 +4178,34 @@
         <f t="shared" si="0"/>
         <v>64.674999999999997</v>
       </c>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="56"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56"/>
-      <c r="Y9" s="56"/>
-      <c r="Z9" s="56"/>
-      <c r="AA9" s="56"/>
-      <c r="AB9" s="56"/>
-      <c r="AC9" s="56"/>
-      <c r="AE9" s="56"/>
-      <c r="AF9" s="56"/>
-      <c r="AI9" s="56"/>
-      <c r="AJ9" s="56"/>
-      <c r="AL9" s="56"/>
-      <c r="AM9" s="56"/>
-      <c r="AN9" s="56"/>
-      <c r="AO9" s="56"/>
-      <c r="AP9" s="56"/>
-      <c r="AQ9" s="56"/>
-      <c r="AR9" s="56"/>
-      <c r="AS9" s="56"/>
-      <c r="AT9" s="56"/>
-      <c r="AU9" s="56"/>
-      <c r="AV9" s="56"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AE9" s="58"/>
+      <c r="AF9" s="58"/>
+      <c r="AI9" s="58"/>
+      <c r="AJ9" s="58"/>
+      <c r="AL9" s="58"/>
+      <c r="AM9" s="58"/>
+      <c r="AN9" s="58"/>
+      <c r="AO9" s="58"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="58"/>
+      <c r="AR9" s="58"/>
+      <c r="AS9" s="58"/>
+      <c r="AT9" s="58"/>
+      <c r="AU9" s="58"/>
+      <c r="AV9" s="58"/>
     </row>
     <row r="10" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
@@ -4249,34 +4235,34 @@
         <f t="shared" si="0"/>
         <v>32.575000000000003</v>
       </c>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="56"/>
-      <c r="W10" s="56"/>
-      <c r="X10" s="56"/>
-      <c r="Y10" s="56"/>
-      <c r="Z10" s="56"/>
-      <c r="AA10" s="56"/>
-      <c r="AB10" s="56"/>
-      <c r="AC10" s="56"/>
-      <c r="AE10" s="56"/>
-      <c r="AF10" s="56"/>
-      <c r="AI10" s="56"/>
-      <c r="AJ10" s="56"/>
-      <c r="AL10" s="56"/>
-      <c r="AM10" s="56"/>
-      <c r="AN10" s="56"/>
-      <c r="AO10" s="56"/>
-      <c r="AP10" s="56"/>
-      <c r="AQ10" s="56"/>
-      <c r="AR10" s="56"/>
-      <c r="AS10" s="56"/>
-      <c r="AT10" s="56"/>
-      <c r="AU10" s="56"/>
-      <c r="AV10" s="56"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="58"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="58"/>
+      <c r="Y10" s="58"/>
+      <c r="Z10" s="58"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AE10" s="58"/>
+      <c r="AF10" s="58"/>
+      <c r="AI10" s="58"/>
+      <c r="AJ10" s="58"/>
+      <c r="AL10" s="58"/>
+      <c r="AM10" s="58"/>
+      <c r="AN10" s="58"/>
+      <c r="AO10" s="58"/>
+      <c r="AP10" s="58"/>
+      <c r="AQ10" s="58"/>
+      <c r="AR10" s="58"/>
+      <c r="AS10" s="58"/>
+      <c r="AT10" s="58"/>
+      <c r="AU10" s="58"/>
+      <c r="AV10" s="58"/>
     </row>
     <row r="11" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
@@ -4302,34 +4288,34 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="Q11" s="56"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="56"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="56"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
-      <c r="Y11" s="56"/>
-      <c r="Z11" s="56"/>
-      <c r="AA11" s="56"/>
-      <c r="AB11" s="56"/>
-      <c r="AC11" s="56"/>
-      <c r="AE11" s="56"/>
-      <c r="AF11" s="56"/>
-      <c r="AI11" s="56"/>
-      <c r="AJ11" s="56"/>
-      <c r="AL11" s="56"/>
-      <c r="AM11" s="56"/>
-      <c r="AN11" s="56"/>
-      <c r="AO11" s="56"/>
-      <c r="AP11" s="56"/>
-      <c r="AQ11" s="56"/>
-      <c r="AR11" s="56"/>
-      <c r="AS11" s="56"/>
-      <c r="AT11" s="56"/>
-      <c r="AU11" s="56"/>
-      <c r="AV11" s="56"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11" s="58"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AL11" s="58"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11" s="58"/>
+      <c r="AO11" s="58"/>
+      <c r="AP11" s="58"/>
+      <c r="AQ11" s="58"/>
+      <c r="AR11" s="58"/>
+      <c r="AS11" s="58"/>
+      <c r="AT11" s="58"/>
+      <c r="AU11" s="58"/>
+      <c r="AV11" s="58"/>
     </row>
     <row r="12" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
@@ -4357,34 +4343,34 @@
         <f t="shared" si="0"/>
         <v>52.70000000000001</v>
       </c>
-      <c r="Q12" s="56"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="56"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="56"/>
-      <c r="Y12" s="56"/>
-      <c r="Z12" s="56"/>
-      <c r="AA12" s="56"/>
-      <c r="AB12" s="56"/>
-      <c r="AC12" s="56"/>
-      <c r="AE12" s="56"/>
-      <c r="AF12" s="56"/>
-      <c r="AI12" s="56"/>
-      <c r="AJ12" s="56"/>
-      <c r="AL12" s="56"/>
-      <c r="AM12" s="56"/>
-      <c r="AN12" s="56"/>
-      <c r="AO12" s="56"/>
-      <c r="AP12" s="56"/>
-      <c r="AQ12" s="56"/>
-      <c r="AR12" s="56"/>
-      <c r="AS12" s="56"/>
-      <c r="AT12" s="56"/>
-      <c r="AU12" s="56"/>
-      <c r="AV12" s="56"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="58"/>
+      <c r="Y12" s="58"/>
+      <c r="Z12" s="58"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AE12" s="58"/>
+      <c r="AF12" s="58"/>
+      <c r="AI12" s="58"/>
+      <c r="AJ12" s="58"/>
+      <c r="AL12" s="58"/>
+      <c r="AM12" s="58"/>
+      <c r="AN12" s="58"/>
+      <c r="AO12" s="58"/>
+      <c r="AP12" s="58"/>
+      <c r="AQ12" s="58"/>
+      <c r="AR12" s="58"/>
+      <c r="AS12" s="58"/>
+      <c r="AT12" s="58"/>
+      <c r="AU12" s="58"/>
+      <c r="AV12" s="58"/>
     </row>
     <row r="13" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
@@ -4414,66 +4400,66 @@
         <f t="shared" si="0"/>
         <v>45.800000000000004</v>
       </c>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="56"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="56"/>
-      <c r="Y13" s="56"/>
-      <c r="Z13" s="56"/>
-      <c r="AA13" s="56"/>
-      <c r="AB13" s="56"/>
-      <c r="AC13" s="56"/>
-      <c r="AE13" s="56"/>
-      <c r="AF13" s="56"/>
-      <c r="AI13" s="56"/>
-      <c r="AJ13" s="56"/>
-      <c r="AL13" s="56"/>
-      <c r="AM13" s="56"/>
-      <c r="AN13" s="56"/>
-      <c r="AO13" s="56"/>
-      <c r="AP13" s="56"/>
-      <c r="AQ13" s="56"/>
-      <c r="AR13" s="56"/>
-      <c r="AS13" s="56"/>
-      <c r="AT13" s="56"/>
-      <c r="AU13" s="56"/>
-      <c r="AV13" s="56"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
+      <c r="Z13" s="58"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AE13" s="58"/>
+      <c r="AF13" s="58"/>
+      <c r="AI13" s="58"/>
+      <c r="AJ13" s="58"/>
+      <c r="AL13" s="58"/>
+      <c r="AM13" s="58"/>
+      <c r="AN13" s="58"/>
+      <c r="AO13" s="58"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="58"/>
+      <c r="AR13" s="58"/>
+      <c r="AS13" s="58"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="58"/>
+      <c r="AV13" s="58"/>
     </row>
     <row r="14" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I14" s="13"/>
       <c r="J14" s="39"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="56"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
-      <c r="Y14" s="56"/>
-      <c r="Z14" s="56"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="56"/>
-      <c r="AC14" s="56"/>
-      <c r="AE14" s="56"/>
-      <c r="AF14" s="56"/>
-      <c r="AI14" s="56"/>
-      <c r="AJ14" s="56"/>
-      <c r="AL14" s="56"/>
-      <c r="AM14" s="56"/>
-      <c r="AN14" s="56"/>
-      <c r="AO14" s="56"/>
-      <c r="AP14" s="56"/>
-      <c r="AQ14" s="56"/>
-      <c r="AR14" s="56"/>
-      <c r="AS14" s="56"/>
-      <c r="AT14" s="56"/>
-      <c r="AU14" s="56"/>
-      <c r="AV14" s="56"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="58"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="58"/>
+      <c r="X14" s="58"/>
+      <c r="Y14" s="58"/>
+      <c r="Z14" s="58"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AE14" s="58"/>
+      <c r="AF14" s="58"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="58"/>
+      <c r="AL14" s="58"/>
+      <c r="AM14" s="58"/>
+      <c r="AN14" s="58"/>
+      <c r="AO14" s="58"/>
+      <c r="AP14" s="58"/>
+      <c r="AQ14" s="58"/>
+      <c r="AR14" s="58"/>
+      <c r="AS14" s="58"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="58"/>
+      <c r="AV14" s="58"/>
     </row>
     <row r="15" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1"/>
@@ -4498,34 +4484,34 @@
       <c r="J15" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="56"/>
-      <c r="Y15" s="56"/>
-      <c r="Z15" s="56"/>
-      <c r="AA15" s="56"/>
-      <c r="AB15" s="56"/>
-      <c r="AC15" s="56"/>
-      <c r="AE15" s="56"/>
-      <c r="AF15" s="56"/>
-      <c r="AI15" s="56"/>
-      <c r="AJ15" s="56"/>
-      <c r="AL15" s="56"/>
-      <c r="AM15" s="56"/>
-      <c r="AN15" s="56"/>
-      <c r="AO15" s="56"/>
-      <c r="AP15" s="56"/>
-      <c r="AQ15" s="56"/>
-      <c r="AR15" s="56"/>
-      <c r="AS15" s="56"/>
-      <c r="AT15" s="56"/>
-      <c r="AU15" s="56"/>
-      <c r="AV15" s="56"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15" s="58"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="58"/>
+      <c r="AC15" s="58"/>
+      <c r="AE15" s="58"/>
+      <c r="AF15" s="58"/>
+      <c r="AI15" s="58"/>
+      <c r="AJ15" s="58"/>
+      <c r="AL15" s="58"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+      <c r="AO15" s="58"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="58"/>
+      <c r="AR15" s="58"/>
+      <c r="AS15" s="58"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="58"/>
+      <c r="AV15" s="58"/>
     </row>
     <row r="16" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="73" t="s">
@@ -4553,34 +4539,34 @@
         <f>SUM(D16:H16)</f>
         <v>1480</v>
       </c>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
-      <c r="Y16" s="56"/>
-      <c r="Z16" s="56"/>
-      <c r="AA16" s="56"/>
-      <c r="AB16" s="56"/>
-      <c r="AC16" s="56"/>
-      <c r="AE16" s="56"/>
-      <c r="AF16" s="56"/>
-      <c r="AI16" s="56"/>
-      <c r="AJ16" s="56"/>
-      <c r="AL16" s="56"/>
-      <c r="AM16" s="56"/>
-      <c r="AN16" s="56"/>
-      <c r="AO16" s="56"/>
-      <c r="AP16" s="56"/>
-      <c r="AQ16" s="56"/>
-      <c r="AR16" s="56"/>
-      <c r="AS16" s="56"/>
-      <c r="AT16" s="56"/>
-      <c r="AU16" s="56"/>
-      <c r="AV16" s="56"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
+      <c r="Y16" s="58"/>
+      <c r="Z16" s="58"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AE16" s="58"/>
+      <c r="AF16" s="58"/>
+      <c r="AI16" s="58"/>
+      <c r="AJ16" s="58"/>
+      <c r="AL16" s="58"/>
+      <c r="AM16" s="58"/>
+      <c r="AN16" s="58"/>
+      <c r="AO16" s="58"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="58"/>
+      <c r="AR16" s="58"/>
+      <c r="AS16" s="58"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="58"/>
+      <c r="AV16" s="58"/>
     </row>
     <row r="17" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="75"/>
@@ -4606,34 +4592,34 @@
         <f>SUM(D17:H17)</f>
         <v>1480</v>
       </c>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
-      <c r="Y17" s="56"/>
-      <c r="Z17" s="56"/>
-      <c r="AA17" s="56"/>
-      <c r="AB17" s="56"/>
-      <c r="AC17" s="56"/>
-      <c r="AE17" s="56"/>
-      <c r="AF17" s="56"/>
-      <c r="AI17" s="56"/>
-      <c r="AJ17" s="56"/>
-      <c r="AL17" s="56"/>
-      <c r="AM17" s="56"/>
-      <c r="AN17" s="56"/>
-      <c r="AO17" s="56"/>
-      <c r="AP17" s="56"/>
-      <c r="AQ17" s="56"/>
-      <c r="AR17" s="56"/>
-      <c r="AS17" s="56"/>
-      <c r="AT17" s="56"/>
-      <c r="AU17" s="56"/>
-      <c r="AV17" s="56"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="58"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
+      <c r="Y17" s="58"/>
+      <c r="Z17" s="58"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AE17" s="58"/>
+      <c r="AF17" s="58"/>
+      <c r="AI17" s="58"/>
+      <c r="AJ17" s="58"/>
+      <c r="AL17" s="58"/>
+      <c r="AM17" s="58"/>
+      <c r="AN17" s="58"/>
+      <c r="AO17" s="58"/>
+      <c r="AP17" s="58"/>
+      <c r="AQ17" s="58"/>
+      <c r="AR17" s="58"/>
+      <c r="AS17" s="58"/>
+      <c r="AT17" s="58"/>
+      <c r="AU17" s="58"/>
+      <c r="AV17" s="58"/>
     </row>
     <row r="18" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="77"/>
@@ -4666,552 +4652,552 @@
         <f>J17-J16</f>
         <v>0</v>
       </c>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="56"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
-      <c r="Y18" s="56"/>
-      <c r="Z18" s="56"/>
-      <c r="AA18" s="56"/>
-      <c r="AB18" s="56"/>
-      <c r="AC18" s="56"/>
-      <c r="AE18" s="56"/>
-      <c r="AF18" s="56"/>
-      <c r="AI18" s="56"/>
-      <c r="AJ18" s="56"/>
-      <c r="AL18" s="56"/>
-      <c r="AM18" s="56"/>
-      <c r="AN18" s="56"/>
-      <c r="AO18" s="56"/>
-      <c r="AP18" s="56"/>
-      <c r="AQ18" s="56"/>
-      <c r="AR18" s="56"/>
-      <c r="AS18" s="56"/>
-      <c r="AT18" s="56"/>
-      <c r="AU18" s="56"/>
-      <c r="AV18" s="56"/>
+      <c r="R18" s="58"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+      <c r="Y18" s="58"/>
+      <c r="Z18" s="58"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AE18" s="58"/>
+      <c r="AF18" s="58"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AL18" s="58"/>
+      <c r="AM18" s="58"/>
+      <c r="AN18" s="58"/>
+      <c r="AO18" s="58"/>
+      <c r="AP18" s="58"/>
+      <c r="AQ18" s="58"/>
+      <c r="AR18" s="58"/>
+      <c r="AS18" s="58"/>
+      <c r="AT18" s="58"/>
+      <c r="AU18" s="58"/>
+      <c r="AV18" s="58"/>
     </row>
     <row r="19" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R19" s="56"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="56"/>
-      <c r="V19" s="56"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
-      <c r="Y19" s="56"/>
-      <c r="Z19" s="56"/>
-      <c r="AA19" s="56"/>
-      <c r="AB19" s="56"/>
-      <c r="AC19" s="56"/>
-      <c r="AE19" s="56"/>
-      <c r="AF19" s="56"/>
-      <c r="AI19" s="56"/>
-      <c r="AJ19" s="56"/>
-      <c r="AL19" s="56"/>
-      <c r="AM19" s="56"/>
-      <c r="AN19" s="56"/>
-      <c r="AO19" s="56"/>
-      <c r="AP19" s="56"/>
-      <c r="AQ19" s="56"/>
-      <c r="AR19" s="56"/>
-      <c r="AS19" s="56"/>
-      <c r="AT19" s="56"/>
-      <c r="AU19" s="56"/>
-      <c r="AV19" s="56"/>
+      <c r="R19" s="58"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="V19" s="58"/>
+      <c r="W19" s="58"/>
+      <c r="X19" s="58"/>
+      <c r="Y19" s="58"/>
+      <c r="Z19" s="58"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AE19" s="58"/>
+      <c r="AF19" s="58"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
+      <c r="AL19" s="58"/>
+      <c r="AM19" s="58"/>
+      <c r="AN19" s="58"/>
+      <c r="AO19" s="58"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="58"/>
+      <c r="AR19" s="58"/>
+      <c r="AS19" s="58"/>
+      <c r="AT19" s="58"/>
+      <c r="AU19" s="58"/>
+      <c r="AV19" s="58"/>
     </row>
     <row r="20" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="V20" s="56"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
-      <c r="Y20" s="56"/>
-      <c r="Z20" s="56"/>
-      <c r="AA20" s="56"/>
-      <c r="AB20" s="56"/>
-      <c r="AC20" s="56"/>
-      <c r="AE20" s="56"/>
-      <c r="AF20" s="56"/>
-      <c r="AI20" s="56"/>
-      <c r="AJ20" s="56"/>
-      <c r="AL20" s="56"/>
-      <c r="AM20" s="56"/>
-      <c r="AN20" s="56"/>
-      <c r="AO20" s="56"/>
-      <c r="AP20" s="56"/>
-      <c r="AQ20" s="56"/>
-      <c r="AR20" s="56"/>
-      <c r="AS20" s="56"/>
-      <c r="AT20" s="56"/>
-      <c r="AU20" s="56"/>
-      <c r="AV20" s="56"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
+      <c r="Y20" s="58"/>
+      <c r="Z20" s="58"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AE20" s="58"/>
+      <c r="AF20" s="58"/>
+      <c r="AI20" s="58"/>
+      <c r="AJ20" s="58"/>
+      <c r="AL20" s="58"/>
+      <c r="AM20" s="58"/>
+      <c r="AN20" s="58"/>
+      <c r="AO20" s="58"/>
+      <c r="AP20" s="58"/>
+      <c r="AQ20" s="58"/>
+      <c r="AR20" s="58"/>
+      <c r="AS20" s="58"/>
+      <c r="AT20" s="58"/>
+      <c r="AU20" s="58"/>
+      <c r="AV20" s="58"/>
     </row>
     <row r="21" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
-      <c r="Y21" s="56"/>
-      <c r="Z21" s="56"/>
-      <c r="AA21" s="56"/>
-      <c r="AB21" s="56"/>
-      <c r="AC21" s="56"/>
-      <c r="AE21" s="56"/>
-      <c r="AF21" s="56"/>
-      <c r="AI21" s="56"/>
-      <c r="AJ21" s="56"/>
-      <c r="AL21" s="56"/>
-      <c r="AM21" s="56"/>
-      <c r="AN21" s="56"/>
-      <c r="AO21" s="56"/>
-      <c r="AP21" s="56"/>
-      <c r="AQ21" s="56"/>
-      <c r="AR21" s="56"/>
-      <c r="AS21" s="56"/>
-      <c r="AT21" s="56"/>
-      <c r="AU21" s="56"/>
-      <c r="AV21" s="56"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+      <c r="Y21" s="58"/>
+      <c r="Z21" s="58"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AE21" s="58"/>
+      <c r="AF21" s="58"/>
+      <c r="AI21" s="58"/>
+      <c r="AJ21" s="58"/>
+      <c r="AL21" s="58"/>
+      <c r="AM21" s="58"/>
+      <c r="AN21" s="58"/>
+      <c r="AO21" s="58"/>
+      <c r="AP21" s="58"/>
+      <c r="AQ21" s="58"/>
+      <c r="AR21" s="58"/>
+      <c r="AS21" s="58"/>
+      <c r="AT21" s="58"/>
+      <c r="AU21" s="58"/>
+      <c r="AV21" s="58"/>
     </row>
     <row r="22" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
-      <c r="Y22" s="56"/>
-      <c r="Z22" s="56"/>
-      <c r="AA22" s="56"/>
-      <c r="AB22" s="56"/>
-      <c r="AC22" s="56"/>
-      <c r="AE22" s="56"/>
-      <c r="AF22" s="56"/>
-      <c r="AI22" s="56"/>
-      <c r="AJ22" s="56"/>
-      <c r="AL22" s="56"/>
-      <c r="AM22" s="56"/>
-      <c r="AN22" s="56"/>
-      <c r="AO22" s="56"/>
-      <c r="AP22" s="56"/>
-      <c r="AQ22" s="56"/>
-      <c r="AR22" s="56"/>
-      <c r="AS22" s="56"/>
-      <c r="AT22" s="56"/>
-      <c r="AU22" s="56"/>
-      <c r="AV22" s="56"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+      <c r="Y22" s="58"/>
+      <c r="Z22" s="58"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58"/>
+      <c r="AC22" s="58"/>
+      <c r="AE22" s="58"/>
+      <c r="AF22" s="58"/>
+      <c r="AI22" s="58"/>
+      <c r="AJ22" s="58"/>
+      <c r="AL22" s="58"/>
+      <c r="AM22" s="58"/>
+      <c r="AN22" s="58"/>
+      <c r="AO22" s="58"/>
+      <c r="AP22" s="58"/>
+      <c r="AQ22" s="58"/>
+      <c r="AR22" s="58"/>
+      <c r="AS22" s="58"/>
+      <c r="AT22" s="58"/>
+      <c r="AU22" s="58"/>
+      <c r="AV22" s="58"/>
     </row>
     <row r="23" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="56"/>
-      <c r="AA23" s="56"/>
-      <c r="AB23" s="56"/>
-      <c r="AC23" s="56"/>
-      <c r="AE23" s="56"/>
-      <c r="AF23" s="56"/>
-      <c r="AI23" s="56"/>
-      <c r="AJ23" s="56"/>
-      <c r="AL23" s="56"/>
-      <c r="AM23" s="56"/>
-      <c r="AN23" s="56"/>
-      <c r="AO23" s="56"/>
-      <c r="AP23" s="56"/>
-      <c r="AQ23" s="56"/>
-      <c r="AR23" s="56"/>
-      <c r="AS23" s="56"/>
-      <c r="AT23" s="56"/>
-      <c r="AU23" s="56"/>
-      <c r="AV23" s="56"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+      <c r="Y23" s="58"/>
+      <c r="Z23" s="58"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="58"/>
+      <c r="AC23" s="58"/>
+      <c r="AE23" s="58"/>
+      <c r="AF23" s="58"/>
+      <c r="AI23" s="58"/>
+      <c r="AJ23" s="58"/>
+      <c r="AL23" s="58"/>
+      <c r="AM23" s="58"/>
+      <c r="AN23" s="58"/>
+      <c r="AO23" s="58"/>
+      <c r="AP23" s="58"/>
+      <c r="AQ23" s="58"/>
+      <c r="AR23" s="58"/>
+      <c r="AS23" s="58"/>
+      <c r="AT23" s="58"/>
+      <c r="AU23" s="58"/>
+      <c r="AV23" s="58"/>
     </row>
     <row r="24" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="56"/>
-      <c r="AA24" s="56"/>
-      <c r="AB24" s="56"/>
-      <c r="AC24" s="56"/>
-      <c r="AE24" s="56"/>
-      <c r="AF24" s="56"/>
-      <c r="AI24" s="56"/>
-      <c r="AJ24" s="56"/>
-      <c r="AL24" s="56"/>
-      <c r="AM24" s="56"/>
-      <c r="AN24" s="56"/>
-      <c r="AO24" s="56"/>
-      <c r="AP24" s="56"/>
-      <c r="AQ24" s="56"/>
-      <c r="AR24" s="56"/>
-      <c r="AS24" s="56"/>
-      <c r="AT24" s="56"/>
-      <c r="AU24" s="56"/>
-      <c r="AV24" s="56"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+      <c r="Y24" s="58"/>
+      <c r="Z24" s="58"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="58"/>
+      <c r="AC24" s="58"/>
+      <c r="AE24" s="58"/>
+      <c r="AF24" s="58"/>
+      <c r="AI24" s="58"/>
+      <c r="AJ24" s="58"/>
+      <c r="AL24" s="58"/>
+      <c r="AM24" s="58"/>
+      <c r="AN24" s="58"/>
+      <c r="AO24" s="58"/>
+      <c r="AP24" s="58"/>
+      <c r="AQ24" s="58"/>
+      <c r="AR24" s="58"/>
+      <c r="AS24" s="58"/>
+      <c r="AT24" s="58"/>
+      <c r="AU24" s="58"/>
+      <c r="AV24" s="58"/>
     </row>
     <row r="25" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="V25" s="56"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
-      <c r="Y25" s="56"/>
-      <c r="Z25" s="56"/>
-      <c r="AA25" s="56"/>
-      <c r="AB25" s="56"/>
-      <c r="AC25" s="56"/>
-      <c r="AE25" s="56"/>
-      <c r="AF25" s="56"/>
-      <c r="AI25" s="56"/>
-      <c r="AJ25" s="56"/>
-      <c r="AL25" s="56"/>
-      <c r="AM25" s="56"/>
-      <c r="AN25" s="56"/>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="56"/>
-      <c r="AQ25" s="56"/>
-      <c r="AR25" s="56"/>
-      <c r="AS25" s="56"/>
-      <c r="AT25" s="56"/>
-      <c r="AU25" s="56"/>
-      <c r="AV25" s="56"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="V25" s="58"/>
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="58"/>
+      <c r="Z25" s="58"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="58"/>
+      <c r="AC25" s="58"/>
+      <c r="AE25" s="58"/>
+      <c r="AF25" s="58"/>
+      <c r="AI25" s="58"/>
+      <c r="AJ25" s="58"/>
+      <c r="AL25" s="58"/>
+      <c r="AM25" s="58"/>
+      <c r="AN25" s="58"/>
+      <c r="AO25" s="58"/>
+      <c r="AP25" s="58"/>
+      <c r="AQ25" s="58"/>
+      <c r="AR25" s="58"/>
+      <c r="AS25" s="58"/>
+      <c r="AT25" s="58"/>
+      <c r="AU25" s="58"/>
+      <c r="AV25" s="58"/>
     </row>
     <row r="26" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="V26" s="56"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
-      <c r="Y26" s="56"/>
-      <c r="Z26" s="56"/>
-      <c r="AA26" s="56"/>
-      <c r="AB26" s="56"/>
-      <c r="AC26" s="56"/>
-      <c r="AE26" s="56"/>
-      <c r="AF26" s="56"/>
-      <c r="AI26" s="56"/>
-      <c r="AJ26" s="56"/>
-      <c r="AL26" s="56"/>
-      <c r="AM26" s="56"/>
-      <c r="AN26" s="56"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="56"/>
-      <c r="AQ26" s="56"/>
-      <c r="AR26" s="56"/>
-      <c r="AS26" s="56"/>
-      <c r="AT26" s="56"/>
-      <c r="AU26" s="56"/>
-      <c r="AV26" s="56"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+      <c r="Y26" s="58"/>
+      <c r="Z26" s="58"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="58"/>
+      <c r="AC26" s="58"/>
+      <c r="AE26" s="58"/>
+      <c r="AF26" s="58"/>
+      <c r="AI26" s="58"/>
+      <c r="AJ26" s="58"/>
+      <c r="AL26" s="58"/>
+      <c r="AM26" s="58"/>
+      <c r="AN26" s="58"/>
+      <c r="AO26" s="58"/>
+      <c r="AP26" s="58"/>
+      <c r="AQ26" s="58"/>
+      <c r="AR26" s="58"/>
+      <c r="AS26" s="58"/>
+      <c r="AT26" s="58"/>
+      <c r="AU26" s="58"/>
+      <c r="AV26" s="58"/>
     </row>
     <row r="27" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="56"/>
-      <c r="Z27" s="56"/>
-      <c r="AA27" s="56"/>
-      <c r="AB27" s="56"/>
-      <c r="AC27" s="56"/>
-      <c r="AE27" s="56"/>
-      <c r="AF27" s="56"/>
-      <c r="AI27" s="56"/>
-      <c r="AJ27" s="56"/>
-      <c r="AL27" s="56"/>
-      <c r="AM27" s="56"/>
-      <c r="AN27" s="56"/>
-      <c r="AO27" s="56"/>
-      <c r="AP27" s="56"/>
-      <c r="AQ27" s="56"/>
-      <c r="AR27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AT27" s="56"/>
-      <c r="AU27" s="56"/>
-      <c r="AV27" s="56"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+      <c r="Y27" s="58"/>
+      <c r="Z27" s="58"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="58"/>
+      <c r="AE27" s="58"/>
+      <c r="AF27" s="58"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="58"/>
+      <c r="AL27" s="58"/>
+      <c r="AM27" s="58"/>
+      <c r="AN27" s="58"/>
+      <c r="AO27" s="58"/>
+      <c r="AP27" s="58"/>
+      <c r="AQ27" s="58"/>
+      <c r="AR27" s="58"/>
+      <c r="AS27" s="58"/>
+      <c r="AT27" s="58"/>
+      <c r="AU27" s="58"/>
+      <c r="AV27" s="58"/>
     </row>
     <row r="28" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="V28" s="56"/>
-      <c r="W28" s="56"/>
-      <c r="X28" s="56"/>
-      <c r="Y28" s="56"/>
-      <c r="Z28" s="56"/>
-      <c r="AA28" s="56"/>
-      <c r="AB28" s="56"/>
-      <c r="AC28" s="56"/>
-      <c r="AE28" s="56"/>
-      <c r="AF28" s="56"/>
-      <c r="AI28" s="56"/>
-      <c r="AJ28" s="56"/>
-      <c r="AL28" s="56"/>
-      <c r="AM28" s="56"/>
-      <c r="AN28" s="56"/>
-      <c r="AO28" s="56"/>
-      <c r="AP28" s="56"/>
-      <c r="AQ28" s="56"/>
-      <c r="AR28" s="56"/>
-      <c r="AS28" s="56"/>
-      <c r="AT28" s="56"/>
-      <c r="AU28" s="56"/>
-      <c r="AV28" s="56"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="V28" s="58"/>
+      <c r="W28" s="58"/>
+      <c r="X28" s="58"/>
+      <c r="Y28" s="58"/>
+      <c r="Z28" s="58"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="58"/>
+      <c r="AC28" s="58"/>
+      <c r="AE28" s="58"/>
+      <c r="AF28" s="58"/>
+      <c r="AI28" s="58"/>
+      <c r="AJ28" s="58"/>
+      <c r="AL28" s="58"/>
+      <c r="AM28" s="58"/>
+      <c r="AN28" s="58"/>
+      <c r="AO28" s="58"/>
+      <c r="AP28" s="58"/>
+      <c r="AQ28" s="58"/>
+      <c r="AR28" s="58"/>
+      <c r="AS28" s="58"/>
+      <c r="AT28" s="58"/>
+      <c r="AU28" s="58"/>
+      <c r="AV28" s="58"/>
     </row>
     <row r="29" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="56"/>
-      <c r="Z29" s="56"/>
-      <c r="AA29" s="56"/>
-      <c r="AB29" s="56"/>
-      <c r="AC29" s="56"/>
-      <c r="AE29" s="56"/>
-      <c r="AF29" s="56"/>
-      <c r="AI29" s="56"/>
-      <c r="AJ29" s="56"/>
-      <c r="AL29" s="56"/>
-      <c r="AM29" s="56"/>
-      <c r="AN29" s="56"/>
-      <c r="AO29" s="56"/>
-      <c r="AP29" s="56"/>
-      <c r="AQ29" s="56"/>
-      <c r="AR29" s="56"/>
-      <c r="AS29" s="56"/>
-      <c r="AT29" s="56"/>
-      <c r="AU29" s="56"/>
-      <c r="AV29" s="56"/>
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="V29" s="58"/>
+      <c r="W29" s="58"/>
+      <c r="X29" s="58"/>
+      <c r="Y29" s="58"/>
+      <c r="Z29" s="58"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="58"/>
+      <c r="AC29" s="58"/>
+      <c r="AE29" s="58"/>
+      <c r="AF29" s="58"/>
+      <c r="AI29" s="58"/>
+      <c r="AJ29" s="58"/>
+      <c r="AL29" s="58"/>
+      <c r="AM29" s="58"/>
+      <c r="AN29" s="58"/>
+      <c r="AO29" s="58"/>
+      <c r="AP29" s="58"/>
+      <c r="AQ29" s="58"/>
+      <c r="AR29" s="58"/>
+      <c r="AS29" s="58"/>
+      <c r="AT29" s="58"/>
+      <c r="AU29" s="58"/>
+      <c r="AV29" s="58"/>
     </row>
     <row r="30" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="V30" s="56"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="56"/>
-      <c r="Y30" s="56"/>
-      <c r="Z30" s="56"/>
-      <c r="AA30" s="56"/>
-      <c r="AB30" s="56"/>
-      <c r="AC30" s="56"/>
-      <c r="AE30" s="56"/>
-      <c r="AF30" s="56"/>
-      <c r="AI30" s="56"/>
-      <c r="AJ30" s="56"/>
-      <c r="AL30" s="56"/>
-      <c r="AM30" s="56"/>
-      <c r="AN30" s="56"/>
-      <c r="AO30" s="56"/>
-      <c r="AP30" s="56"/>
-      <c r="AQ30" s="56"/>
-      <c r="AR30" s="56"/>
-      <c r="AS30" s="56"/>
-      <c r="AT30" s="56"/>
-      <c r="AU30" s="56"/>
-      <c r="AV30" s="56"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
+      <c r="V30" s="58"/>
+      <c r="W30" s="58"/>
+      <c r="X30" s="58"/>
+      <c r="Y30" s="58"/>
+      <c r="Z30" s="58"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="58"/>
+      <c r="AC30" s="58"/>
+      <c r="AE30" s="58"/>
+      <c r="AF30" s="58"/>
+      <c r="AI30" s="58"/>
+      <c r="AJ30" s="58"/>
+      <c r="AL30" s="58"/>
+      <c r="AM30" s="58"/>
+      <c r="AN30" s="58"/>
+      <c r="AO30" s="58"/>
+      <c r="AP30" s="58"/>
+      <c r="AQ30" s="58"/>
+      <c r="AR30" s="58"/>
+      <c r="AS30" s="58"/>
+      <c r="AT30" s="58"/>
+      <c r="AU30" s="58"/>
+      <c r="AV30" s="58"/>
     </row>
     <row r="31" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="T31" s="56"/>
-      <c r="U31" s="56"/>
-      <c r="V31" s="56"/>
-      <c r="W31" s="56"/>
-      <c r="X31" s="56"/>
-      <c r="Y31" s="56"/>
-      <c r="Z31" s="56"/>
-      <c r="AA31" s="56"/>
-      <c r="AB31" s="56"/>
-      <c r="AC31" s="56"/>
-      <c r="AE31" s="56"/>
-      <c r="AF31" s="56"/>
-      <c r="AI31" s="56"/>
-      <c r="AJ31" s="56"/>
-      <c r="AL31" s="56"/>
-      <c r="AM31" s="56"/>
-      <c r="AN31" s="56"/>
-      <c r="AO31" s="56"/>
-      <c r="AP31" s="56"/>
-      <c r="AQ31" s="56"/>
-      <c r="AR31" s="56"/>
-      <c r="AS31" s="56"/>
-      <c r="AT31" s="56"/>
-      <c r="AU31" s="56"/>
-      <c r="AV31" s="56"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="58"/>
+      <c r="U31" s="58"/>
+      <c r="V31" s="58"/>
+      <c r="W31" s="58"/>
+      <c r="X31" s="58"/>
+      <c r="Y31" s="58"/>
+      <c r="Z31" s="58"/>
+      <c r="AA31" s="58"/>
+      <c r="AB31" s="58"/>
+      <c r="AC31" s="58"/>
+      <c r="AE31" s="58"/>
+      <c r="AF31" s="58"/>
+      <c r="AI31" s="58"/>
+      <c r="AJ31" s="58"/>
+      <c r="AL31" s="58"/>
+      <c r="AM31" s="58"/>
+      <c r="AN31" s="58"/>
+      <c r="AO31" s="58"/>
+      <c r="AP31" s="58"/>
+      <c r="AQ31" s="58"/>
+      <c r="AR31" s="58"/>
+      <c r="AS31" s="58"/>
+      <c r="AT31" s="58"/>
+      <c r="AU31" s="58"/>
+      <c r="AV31" s="58"/>
     </row>
     <row r="32" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T32" s="56"/>
-      <c r="U32" s="56"/>
-      <c r="V32" s="56"/>
-      <c r="W32" s="56"/>
-      <c r="X32" s="56"/>
-      <c r="Y32" s="56"/>
-      <c r="Z32" s="56"/>
-      <c r="AA32" s="56"/>
-      <c r="AB32" s="56"/>
-      <c r="AC32" s="56"/>
-      <c r="AE32" s="56"/>
-      <c r="AF32" s="56"/>
-      <c r="AI32" s="56"/>
-      <c r="AJ32" s="56"/>
-      <c r="AL32" s="56"/>
-      <c r="AM32" s="56"/>
-      <c r="AN32" s="56"/>
-      <c r="AO32" s="56"/>
-      <c r="AP32" s="56"/>
-      <c r="AQ32" s="56"/>
-      <c r="AR32" s="56"/>
-      <c r="AS32" s="56"/>
-      <c r="AT32" s="56"/>
-      <c r="AU32" s="56"/>
-      <c r="AV32" s="56"/>
+      <c r="T32" s="58"/>
+      <c r="U32" s="58"/>
+      <c r="V32" s="58"/>
+      <c r="W32" s="58"/>
+      <c r="X32" s="58"/>
+      <c r="Y32" s="58"/>
+      <c r="Z32" s="58"/>
+      <c r="AA32" s="58"/>
+      <c r="AB32" s="58"/>
+      <c r="AC32" s="58"/>
+      <c r="AE32" s="58"/>
+      <c r="AF32" s="58"/>
+      <c r="AI32" s="58"/>
+      <c r="AJ32" s="58"/>
+      <c r="AL32" s="58"/>
+      <c r="AM32" s="58"/>
+      <c r="AN32" s="58"/>
+      <c r="AO32" s="58"/>
+      <c r="AP32" s="58"/>
+      <c r="AQ32" s="58"/>
+      <c r="AR32" s="58"/>
+      <c r="AS32" s="58"/>
+      <c r="AT32" s="58"/>
+      <c r="AU32" s="58"/>
+      <c r="AV32" s="58"/>
     </row>
     <row r="33" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T33" s="56"/>
-      <c r="U33" s="56"/>
-      <c r="V33" s="56"/>
-      <c r="W33" s="56"/>
-      <c r="X33" s="56"/>
-      <c r="Y33" s="56"/>
-      <c r="Z33" s="56"/>
-      <c r="AA33" s="56"/>
-      <c r="AB33" s="56"/>
-      <c r="AC33" s="56"/>
-      <c r="AE33" s="56"/>
-      <c r="AF33" s="56"/>
-      <c r="AI33" s="56"/>
-      <c r="AJ33" s="56"/>
-      <c r="AL33" s="56"/>
-      <c r="AM33" s="56"/>
-      <c r="AN33" s="56"/>
-      <c r="AO33" s="56"/>
-      <c r="AP33" s="56"/>
-      <c r="AQ33" s="56"/>
-      <c r="AR33" s="56"/>
-      <c r="AS33" s="56"/>
-      <c r="AT33" s="56"/>
-      <c r="AU33" s="56"/>
-      <c r="AV33" s="56"/>
+      <c r="T33" s="58"/>
+      <c r="U33" s="58"/>
+      <c r="V33" s="58"/>
+      <c r="W33" s="58"/>
+      <c r="X33" s="58"/>
+      <c r="Y33" s="58"/>
+      <c r="Z33" s="58"/>
+      <c r="AA33" s="58"/>
+      <c r="AB33" s="58"/>
+      <c r="AC33" s="58"/>
+      <c r="AE33" s="58"/>
+      <c r="AF33" s="58"/>
+      <c r="AI33" s="58"/>
+      <c r="AJ33" s="58"/>
+      <c r="AL33" s="58"/>
+      <c r="AM33" s="58"/>
+      <c r="AN33" s="58"/>
+      <c r="AO33" s="58"/>
+      <c r="AP33" s="58"/>
+      <c r="AQ33" s="58"/>
+      <c r="AR33" s="58"/>
+      <c r="AS33" s="58"/>
+      <c r="AT33" s="58"/>
+      <c r="AU33" s="58"/>
+      <c r="AV33" s="58"/>
     </row>
     <row r="34" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T34" s="56"/>
-      <c r="U34" s="56"/>
-      <c r="V34" s="56"/>
-      <c r="W34" s="56"/>
-      <c r="X34" s="56"/>
-      <c r="Y34" s="56"/>
-      <c r="Z34" s="56"/>
-      <c r="AA34" s="56"/>
-      <c r="AB34" s="56"/>
-      <c r="AC34" s="56"/>
-      <c r="AE34" s="56"/>
-      <c r="AF34" s="56"/>
-      <c r="AI34" s="56"/>
-      <c r="AJ34" s="56"/>
-      <c r="AL34" s="56"/>
-      <c r="AM34" s="56"/>
-      <c r="AN34" s="56"/>
-      <c r="AO34" s="56"/>
-      <c r="AP34" s="56"/>
-      <c r="AQ34" s="56"/>
-      <c r="AR34" s="56"/>
-      <c r="AS34" s="56"/>
-      <c r="AT34" s="56"/>
-      <c r="AU34" s="56"/>
-      <c r="AV34" s="56"/>
+      <c r="T34" s="58"/>
+      <c r="U34" s="58"/>
+      <c r="V34" s="58"/>
+      <c r="W34" s="58"/>
+      <c r="X34" s="58"/>
+      <c r="Y34" s="58"/>
+      <c r="Z34" s="58"/>
+      <c r="AA34" s="58"/>
+      <c r="AB34" s="58"/>
+      <c r="AC34" s="58"/>
+      <c r="AE34" s="58"/>
+      <c r="AF34" s="58"/>
+      <c r="AI34" s="58"/>
+      <c r="AJ34" s="58"/>
+      <c r="AL34" s="58"/>
+      <c r="AM34" s="58"/>
+      <c r="AN34" s="58"/>
+      <c r="AO34" s="58"/>
+      <c r="AP34" s="58"/>
+      <c r="AQ34" s="58"/>
+      <c r="AR34" s="58"/>
+      <c r="AS34" s="58"/>
+      <c r="AT34" s="58"/>
+      <c r="AU34" s="58"/>
+      <c r="AV34" s="58"/>
     </row>
     <row r="35" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T35" s="56"/>
-      <c r="U35" s="56"/>
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
-      <c r="X35" s="56"/>
-      <c r="Y35" s="56"/>
-      <c r="Z35" s="56"/>
-      <c r="AA35" s="56"/>
-      <c r="AB35" s="56"/>
-      <c r="AC35" s="56"/>
-      <c r="AE35" s="56"/>
-      <c r="AF35" s="56"/>
-      <c r="AI35" s="56"/>
-      <c r="AJ35" s="56"/>
-      <c r="AL35" s="56"/>
-      <c r="AM35" s="56"/>
-      <c r="AN35" s="56"/>
-      <c r="AO35" s="56"/>
-      <c r="AP35" s="56"/>
-      <c r="AQ35" s="56"/>
-      <c r="AR35" s="56"/>
-      <c r="AS35" s="56"/>
-      <c r="AT35" s="56"/>
-      <c r="AU35" s="56"/>
-      <c r="AV35" s="56"/>
+      <c r="T35" s="58"/>
+      <c r="U35" s="58"/>
+      <c r="V35" s="58"/>
+      <c r="W35" s="58"/>
+      <c r="X35" s="58"/>
+      <c r="Y35" s="58"/>
+      <c r="Z35" s="58"/>
+      <c r="AA35" s="58"/>
+      <c r="AB35" s="58"/>
+      <c r="AC35" s="58"/>
+      <c r="AE35" s="58"/>
+      <c r="AF35" s="58"/>
+      <c r="AI35" s="58"/>
+      <c r="AJ35" s="58"/>
+      <c r="AL35" s="58"/>
+      <c r="AM35" s="58"/>
+      <c r="AN35" s="58"/>
+      <c r="AO35" s="58"/>
+      <c r="AP35" s="58"/>
+      <c r="AQ35" s="58"/>
+      <c r="AR35" s="58"/>
+      <c r="AS35" s="58"/>
+      <c r="AT35" s="58"/>
+      <c r="AU35" s="58"/>
+      <c r="AV35" s="58"/>
     </row>
     <row r="36" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="X36" s="56"/>
-      <c r="AJ36" s="56"/>
-      <c r="AL36" s="56"/>
-      <c r="AM36" s="56"/>
-      <c r="AN36" s="56"/>
-      <c r="AO36" s="56"/>
-      <c r="AP36" s="56"/>
-      <c r="AQ36" s="56"/>
-      <c r="AR36" s="56"/>
-      <c r="AS36" s="56"/>
-      <c r="AT36" s="56"/>
-      <c r="AU36" s="56"/>
-      <c r="AV36" s="56"/>
+      <c r="Q36" s="58"/>
+      <c r="T36" s="58"/>
+      <c r="U36" s="58"/>
+      <c r="X36" s="58"/>
+      <c r="AJ36" s="58"/>
+      <c r="AL36" s="58"/>
+      <c r="AM36" s="58"/>
+      <c r="AN36" s="58"/>
+      <c r="AO36" s="58"/>
+      <c r="AP36" s="58"/>
+      <c r="AQ36" s="58"/>
+      <c r="AR36" s="58"/>
+      <c r="AS36" s="58"/>
+      <c r="AT36" s="58"/>
+      <c r="AU36" s="58"/>
+      <c r="AV36" s="58"/>
     </row>
     <row r="37" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q37" s="56"/>
-      <c r="T37" s="56"/>
-      <c r="U37" s="56"/>
-      <c r="X37" s="56"/>
-      <c r="AJ37" s="56"/>
-      <c r="AL37" s="56"/>
-      <c r="AM37" s="56"/>
-      <c r="AN37" s="56"/>
-      <c r="AO37" s="56"/>
-      <c r="AP37" s="56"/>
-      <c r="AQ37" s="56"/>
-      <c r="AR37" s="56"/>
-      <c r="AS37" s="56"/>
-      <c r="AT37" s="56"/>
-      <c r="AU37" s="56"/>
-      <c r="AV37" s="56"/>
+      <c r="Q37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="X37" s="58"/>
+      <c r="AJ37" s="58"/>
+      <c r="AL37" s="58"/>
+      <c r="AM37" s="58"/>
+      <c r="AN37" s="58"/>
+      <c r="AO37" s="58"/>
+      <c r="AP37" s="58"/>
+      <c r="AQ37" s="58"/>
+      <c r="AR37" s="58"/>
+      <c r="AS37" s="58"/>
+      <c r="AT37" s="58"/>
+      <c r="AU37" s="58"/>
+      <c r="AV37" s="58"/>
     </row>
     <row r="38" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q38" s="56"/>
-      <c r="T38" s="56"/>
-      <c r="U38" s="56"/>
-      <c r="X38" s="56"/>
-      <c r="AJ38" s="56"/>
-      <c r="AL38" s="56"/>
-      <c r="AM38" s="56"/>
-      <c r="AN38" s="56"/>
-      <c r="AO38" s="56"/>
-      <c r="AP38" s="56"/>
-      <c r="AQ38" s="56"/>
-      <c r="AR38" s="56"/>
-      <c r="AS38" s="56"/>
-      <c r="AT38" s="56"/>
-      <c r="AU38" s="56"/>
-      <c r="AV38" s="56"/>
+      <c r="Q38" s="58"/>
+      <c r="T38" s="58"/>
+      <c r="U38" s="58"/>
+      <c r="X38" s="58"/>
+      <c r="AJ38" s="58"/>
+      <c r="AL38" s="58"/>
+      <c r="AM38" s="58"/>
+      <c r="AN38" s="58"/>
+      <c r="AO38" s="58"/>
+      <c r="AP38" s="58"/>
+      <c r="AQ38" s="58"/>
+      <c r="AR38" s="58"/>
+      <c r="AS38" s="58"/>
+      <c r="AT38" s="58"/>
+      <c r="AU38" s="58"/>
+      <c r="AV38" s="58"/>
     </row>
     <row r="39" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5336,85 +5322,85 @@
       </c>
     </row>
     <row r="53" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL53" s="56"/>
-      <c r="AM53" s="56"/>
-      <c r="AN53" s="56"/>
+      <c r="AL53" s="58"/>
+      <c r="AM53" s="58"/>
+      <c r="AN53" s="58"/>
     </row>
     <row r="54" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL54" s="56"/>
-      <c r="AM54" s="56"/>
-      <c r="AN54" s="56"/>
+      <c r="AL54" s="58"/>
+      <c r="AM54" s="58"/>
+      <c r="AN54" s="58"/>
     </row>
     <row r="55" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL55" s="56"/>
-      <c r="AM55" s="56"/>
-      <c r="AN55" s="56"/>
+      <c r="AL55" s="58"/>
+      <c r="AM55" s="58"/>
+      <c r="AN55" s="58"/>
     </row>
     <row r="56" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL56" s="56"/>
-      <c r="AM56" s="56"/>
-      <c r="AN56" s="56"/>
+      <c r="AL56" s="58"/>
+      <c r="AM56" s="58"/>
+      <c r="AN56" s="58"/>
     </row>
     <row r="57" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL57" s="56"/>
-      <c r="AM57" s="56"/>
-      <c r="AN57" s="56"/>
+      <c r="AL57" s="58"/>
+      <c r="AM57" s="58"/>
+      <c r="AN57" s="58"/>
     </row>
     <row r="60" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K60" s="56"/>
-      <c r="AE60" s="56"/>
-      <c r="AF60" s="56"/>
-      <c r="AI60" s="56"/>
-      <c r="AJ60" s="56"/>
+      <c r="K60" s="58"/>
+      <c r="AE60" s="58"/>
+      <c r="AF60" s="58"/>
+      <c r="AI60" s="58"/>
+      <c r="AJ60" s="58"/>
     </row>
     <row r="61" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K61" s="56"/>
-      <c r="AE61" s="56"/>
-      <c r="AF61" s="56"/>
-      <c r="AI61" s="56"/>
-      <c r="AJ61" s="56"/>
+      <c r="K61" s="58"/>
+      <c r="AE61" s="58"/>
+      <c r="AF61" s="58"/>
+      <c r="AI61" s="58"/>
+      <c r="AJ61" s="58"/>
     </row>
     <row r="62" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y62" s="56"/>
-      <c r="AL62" s="56"/>
-      <c r="AM62" s="56"/>
-      <c r="AN62" s="56"/>
-      <c r="AO62" s="56"/>
-      <c r="AP62" s="56"/>
-      <c r="AQ62" s="56"/>
-      <c r="AR62" s="56"/>
-      <c r="AS62" s="56"/>
-      <c r="AT62" s="56"/>
-      <c r="AU62" s="56"/>
-      <c r="AV62" s="56"/>
+      <c r="Y62" s="58"/>
+      <c r="AL62" s="58"/>
+      <c r="AM62" s="58"/>
+      <c r="AN62" s="58"/>
+      <c r="AO62" s="58"/>
+      <c r="AP62" s="58"/>
+      <c r="AQ62" s="58"/>
+      <c r="AR62" s="58"/>
+      <c r="AS62" s="58"/>
+      <c r="AT62" s="58"/>
+      <c r="AU62" s="58"/>
+      <c r="AV62" s="58"/>
     </row>
     <row r="63" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y63" s="56"/>
-      <c r="AL63" s="56"/>
-      <c r="AM63" s="56"/>
-      <c r="AN63" s="56"/>
-      <c r="AO63" s="56"/>
-      <c r="AP63" s="56"/>
-      <c r="AQ63" s="56"/>
-      <c r="AR63" s="56"/>
-      <c r="AS63" s="56"/>
-      <c r="AT63" s="56"/>
-      <c r="AU63" s="56"/>
-      <c r="AV63" s="56"/>
+      <c r="Y63" s="58"/>
+      <c r="AL63" s="58"/>
+      <c r="AM63" s="58"/>
+      <c r="AN63" s="58"/>
+      <c r="AO63" s="58"/>
+      <c r="AP63" s="58"/>
+      <c r="AQ63" s="58"/>
+      <c r="AR63" s="58"/>
+      <c r="AS63" s="58"/>
+      <c r="AT63" s="58"/>
+      <c r="AU63" s="58"/>
+      <c r="AV63" s="58"/>
     </row>
     <row r="64" spans="11:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y64" s="56"/>
-      <c r="AL64" s="56"/>
-      <c r="AM64" s="56"/>
-      <c r="AN64" s="56"/>
-      <c r="AO64" s="56"/>
-      <c r="AP64" s="56"/>
-      <c r="AQ64" s="56"/>
-      <c r="AR64" s="56"/>
-      <c r="AS64" s="56"/>
-      <c r="AT64" s="56"/>
-      <c r="AU64" s="56"/>
-      <c r="AV64" s="56"/>
+      <c r="Y64" s="58"/>
+      <c r="AL64" s="58"/>
+      <c r="AM64" s="58"/>
+      <c r="AN64" s="58"/>
+      <c r="AO64" s="58"/>
+      <c r="AP64" s="58"/>
+      <c r="AQ64" s="58"/>
+      <c r="AR64" s="58"/>
+      <c r="AS64" s="58"/>
+      <c r="AT64" s="58"/>
+      <c r="AU64" s="58"/>
+      <c r="AV64" s="58"/>
     </row>
     <row r="65" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="1"/>
@@ -5427,54 +5413,54 @@
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
-      <c r="Y65" s="56"/>
-      <c r="AL65" s="56"/>
-      <c r="AM65" s="56"/>
-      <c r="AN65" s="56"/>
-      <c r="AO65" s="56"/>
-      <c r="AP65" s="56"/>
-      <c r="AQ65" s="56"/>
-      <c r="AR65" s="56"/>
-      <c r="AS65" s="56"/>
-      <c r="AT65" s="56"/>
-      <c r="AU65" s="56"/>
-      <c r="AV65" s="56"/>
+      <c r="Y65" s="58"/>
+      <c r="AL65" s="58"/>
+      <c r="AM65" s="58"/>
+      <c r="AN65" s="58"/>
+      <c r="AO65" s="58"/>
+      <c r="AP65" s="58"/>
+      <c r="AQ65" s="58"/>
+      <c r="AR65" s="58"/>
+      <c r="AS65" s="58"/>
+      <c r="AT65" s="58"/>
+      <c r="AU65" s="58"/>
+      <c r="AV65" s="58"/>
     </row>
     <row r="66" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
-      <c r="D66" s="59" t="s">
+      <c r="D66" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="60" t="s">
+      <c r="E66" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="F66" s="60" t="s">
+      <c r="F66" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="G66" s="60" t="s">
+      <c r="G66" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H66" s="61" t="s">
+      <c r="H66" s="63" t="s">
         <v>11</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Y66" s="56"/>
-      <c r="AL66" s="56"/>
-      <c r="AM66" s="56"/>
-      <c r="AN66" s="56"/>
-      <c r="AO66" s="56"/>
-      <c r="AP66" s="56"/>
-      <c r="AQ66" s="56"/>
-      <c r="AR66" s="56"/>
-      <c r="AS66" s="56"/>
-      <c r="AT66" s="56"/>
-      <c r="AU66" s="56"/>
-      <c r="AV66" s="56"/>
+      <c r="Y66" s="58"/>
+      <c r="AL66" s="58"/>
+      <c r="AM66" s="58"/>
+      <c r="AN66" s="58"/>
+      <c r="AO66" s="58"/>
+      <c r="AP66" s="58"/>
+      <c r="AQ66" s="58"/>
+      <c r="AR66" s="58"/>
+      <c r="AS66" s="58"/>
+      <c r="AT66" s="58"/>
+      <c r="AU66" s="58"/>
+      <c r="AV66" s="58"/>
     </row>
     <row r="67" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="79" t="s">
@@ -5484,43 +5470,43 @@
       <c r="C67" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="62">
+      <c r="D67" s="64">
         <f>D68/D16</f>
         <v>4.335</v>
       </c>
-      <c r="E67" s="62">
+      <c r="E67" s="64">
         <f>E68/E16</f>
         <v>1.2313513513513514</v>
       </c>
-      <c r="F67" s="62">
+      <c r="F67" s="64">
         <f>F68/F16</f>
         <v>1.0337837837837838</v>
       </c>
-      <c r="G67" s="62">
+      <c r="G67" s="64">
         <f>G68/G16</f>
         <v>1.0337837837837838</v>
       </c>
-      <c r="H67" s="62" t="e">
+      <c r="H67" s="64" t="e">
         <f>H68/H16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I67" s="63"/>
-      <c r="J67" s="62">
+      <c r="I67" s="65"/>
+      <c r="J67" s="64">
         <f>J68/J16</f>
         <v>1.3915878378378379</v>
       </c>
-      <c r="Y67" s="56"/>
-      <c r="AL67" s="56"/>
-      <c r="AM67" s="56"/>
-      <c r="AN67" s="56"/>
-      <c r="AO67" s="56"/>
-      <c r="AP67" s="56"/>
-      <c r="AQ67" s="56"/>
-      <c r="AR67" s="56"/>
-      <c r="AS67" s="56"/>
-      <c r="AT67" s="56"/>
-      <c r="AU67" s="56"/>
-      <c r="AV67" s="56"/>
+      <c r="Y67" s="58"/>
+      <c r="AL67" s="58"/>
+      <c r="AM67" s="58"/>
+      <c r="AN67" s="58"/>
+      <c r="AO67" s="58"/>
+      <c r="AP67" s="58"/>
+      <c r="AQ67" s="58"/>
+      <c r="AR67" s="58"/>
+      <c r="AS67" s="58"/>
+      <c r="AT67" s="58"/>
+      <c r="AU67" s="58"/>
+      <c r="AV67" s="58"/>
     </row>
     <row r="68" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="75"/>
@@ -5528,38 +5514,38 @@
       <c r="C68" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D68" s="64">
+      <c r="D68" s="66">
         <v>1603.95</v>
       </c>
-      <c r="E68" s="64">
+      <c r="E68" s="66">
         <v>455.6</v>
       </c>
-      <c r="F68" s="64">
+      <c r="F68" s="66">
         <v>382.5</v>
       </c>
-      <c r="G68" s="64">
+      <c r="G68" s="66">
         <v>382.5</v>
       </c>
-      <c r="H68" s="65">
+      <c r="H68" s="67">
         <v>0</v>
       </c>
       <c r="I68" s="1"/>
-      <c r="J68" s="66">
+      <c r="J68" s="68">
         <f>D68+E68</f>
         <v>2059.5500000000002</v>
       </c>
-      <c r="Y68" s="56"/>
-      <c r="AL68" s="56"/>
-      <c r="AM68" s="56"/>
-      <c r="AN68" s="56"/>
-      <c r="AO68" s="56"/>
-      <c r="AP68" s="56"/>
-      <c r="AQ68" s="56"/>
-      <c r="AR68" s="56"/>
-      <c r="AS68" s="56"/>
-      <c r="AT68" s="56"/>
-      <c r="AU68" s="56"/>
-      <c r="AV68" s="56"/>
+      <c r="Y68" s="58"/>
+      <c r="AL68" s="58"/>
+      <c r="AM68" s="58"/>
+      <c r="AN68" s="58"/>
+      <c r="AO68" s="58"/>
+      <c r="AP68" s="58"/>
+      <c r="AQ68" s="58"/>
+      <c r="AR68" s="58"/>
+      <c r="AS68" s="58"/>
+      <c r="AT68" s="58"/>
+      <c r="AU68" s="58"/>
+      <c r="AV68" s="58"/>
     </row>
     <row r="69" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="75"/>
@@ -5571,39 +5557,39 @@
         <f>D68/D17</f>
         <v>4.335</v>
       </c>
-      <c r="E69" s="67">
+      <c r="E69" s="69">
         <f>E68/E17</f>
         <v>1.2313513513513514</v>
       </c>
-      <c r="F69" s="67">
+      <c r="F69" s="69">
         <f>F68/F17</f>
         <v>1.0337837837837838</v>
       </c>
-      <c r="G69" s="67">
+      <c r="G69" s="69">
         <f>G68/G17</f>
         <v>1.0337837837837838</v>
       </c>
-      <c r="H69" s="67" t="e">
+      <c r="H69" s="69" t="e">
         <f>H68/H17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I69" s="63"/>
-      <c r="J69" s="68">
+      <c r="I69" s="65"/>
+      <c r="J69" s="70">
         <f>J68/J17</f>
         <v>1.3915878378378379</v>
       </c>
-      <c r="Y69" s="56"/>
-      <c r="AL69" s="56"/>
-      <c r="AM69" s="56"/>
-      <c r="AN69" s="56"/>
-      <c r="AO69" s="56"/>
-      <c r="AP69" s="56"/>
-      <c r="AQ69" s="56"/>
-      <c r="AR69" s="56"/>
-      <c r="AS69" s="56"/>
-      <c r="AT69" s="56"/>
-      <c r="AU69" s="56"/>
-      <c r="AV69" s="56"/>
+      <c r="Y69" s="58"/>
+      <c r="AL69" s="58"/>
+      <c r="AM69" s="58"/>
+      <c r="AN69" s="58"/>
+      <c r="AO69" s="58"/>
+      <c r="AP69" s="58"/>
+      <c r="AQ69" s="58"/>
+      <c r="AR69" s="58"/>
+      <c r="AS69" s="58"/>
+      <c r="AT69" s="58"/>
+      <c r="AU69" s="58"/>
+      <c r="AV69" s="58"/>
     </row>
     <row r="70" spans="1:48" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="80"/>
@@ -5611,402 +5597,402 @@
       <c r="C70" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D70" s="69">
+      <c r="D70" s="71">
         <f>D67-D69</f>
         <v>0</v>
       </c>
-      <c r="E70" s="69">
+      <c r="E70" s="71">
         <f>E67-E69</f>
         <v>0</v>
       </c>
-      <c r="F70" s="69">
+      <c r="F70" s="71">
         <f>F67-F69</f>
         <v>0</v>
       </c>
-      <c r="G70" s="69">
+      <c r="G70" s="71">
         <f>G67-G69</f>
         <v>0</v>
       </c>
-      <c r="H70" s="70" t="e">
+      <c r="H70" s="72" t="e">
         <f>H67-H69</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I70" s="63"/>
-      <c r="J70" s="68">
+      <c r="I70" s="65"/>
+      <c r="J70" s="70">
         <f>J67-J69</f>
         <v>0</v>
       </c>
-      <c r="Y70" s="56"/>
-      <c r="AL70" s="56"/>
-      <c r="AM70" s="56"/>
-      <c r="AN70" s="56"/>
-      <c r="AO70" s="56"/>
-      <c r="AP70" s="56"/>
-      <c r="AQ70" s="56"/>
-      <c r="AR70" s="56"/>
-      <c r="AS70" s="56"/>
-      <c r="AT70" s="56"/>
-      <c r="AU70" s="56"/>
-      <c r="AV70" s="56"/>
+      <c r="Y70" s="58"/>
+      <c r="AL70" s="58"/>
+      <c r="AM70" s="58"/>
+      <c r="AN70" s="58"/>
+      <c r="AO70" s="58"/>
+      <c r="AP70" s="58"/>
+      <c r="AQ70" s="58"/>
+      <c r="AR70" s="58"/>
+      <c r="AS70" s="58"/>
+      <c r="AT70" s="58"/>
+      <c r="AU70" s="58"/>
+      <c r="AV70" s="58"/>
     </row>
     <row r="71" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y71" s="56"/>
-      <c r="AL71" s="56"/>
-      <c r="AM71" s="56"/>
-      <c r="AN71" s="56"/>
-      <c r="AO71" s="56"/>
-      <c r="AP71" s="56"/>
-      <c r="AQ71" s="56"/>
-      <c r="AR71" s="56"/>
-      <c r="AS71" s="56"/>
-      <c r="AT71" s="56"/>
-      <c r="AU71" s="56"/>
-      <c r="AV71" s="56"/>
+      <c r="Y71" s="58"/>
+      <c r="AL71" s="58"/>
+      <c r="AM71" s="58"/>
+      <c r="AN71" s="58"/>
+      <c r="AO71" s="58"/>
+      <c r="AP71" s="58"/>
+      <c r="AQ71" s="58"/>
+      <c r="AR71" s="58"/>
+      <c r="AS71" s="58"/>
+      <c r="AT71" s="58"/>
+      <c r="AU71" s="58"/>
+      <c r="AV71" s="58"/>
     </row>
     <row r="72" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y72" s="56"/>
-      <c r="AL72" s="56"/>
-      <c r="AM72" s="56"/>
-      <c r="AN72" s="56"/>
-      <c r="AO72" s="56"/>
-      <c r="AP72" s="56"/>
-      <c r="AQ72" s="56"/>
-      <c r="AR72" s="56"/>
-      <c r="AS72" s="56"/>
-      <c r="AT72" s="56"/>
-      <c r="AU72" s="56"/>
-      <c r="AV72" s="56"/>
+      <c r="Y72" s="58"/>
+      <c r="AL72" s="58"/>
+      <c r="AM72" s="58"/>
+      <c r="AN72" s="58"/>
+      <c r="AO72" s="58"/>
+      <c r="AP72" s="58"/>
+      <c r="AQ72" s="58"/>
+      <c r="AR72" s="58"/>
+      <c r="AS72" s="58"/>
+      <c r="AT72" s="58"/>
+      <c r="AU72" s="58"/>
+      <c r="AV72" s="58"/>
     </row>
     <row r="73" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y73" s="56"/>
-      <c r="AL73" s="56"/>
-      <c r="AM73" s="56"/>
-      <c r="AN73" s="56"/>
-      <c r="AO73" s="56"/>
-      <c r="AP73" s="56"/>
-      <c r="AQ73" s="56"/>
-      <c r="AR73" s="56"/>
-      <c r="AS73" s="56"/>
-      <c r="AT73" s="56"/>
-      <c r="AU73" s="56"/>
-      <c r="AV73" s="56"/>
+      <c r="Y73" s="58"/>
+      <c r="AL73" s="58"/>
+      <c r="AM73" s="58"/>
+      <c r="AN73" s="58"/>
+      <c r="AO73" s="58"/>
+      <c r="AP73" s="58"/>
+      <c r="AQ73" s="58"/>
+      <c r="AR73" s="58"/>
+      <c r="AS73" s="58"/>
+      <c r="AT73" s="58"/>
+      <c r="AU73" s="58"/>
+      <c r="AV73" s="58"/>
     </row>
     <row r="74" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y74" s="56"/>
-      <c r="AL74" s="56"/>
-      <c r="AM74" s="56"/>
-      <c r="AN74" s="56"/>
-      <c r="AO74" s="56"/>
-      <c r="AP74" s="56"/>
-      <c r="AQ74" s="56"/>
-      <c r="AR74" s="56"/>
-      <c r="AS74" s="56"/>
-      <c r="AT74" s="56"/>
-      <c r="AU74" s="56"/>
-      <c r="AV74" s="56"/>
+      <c r="Y74" s="58"/>
+      <c r="AL74" s="58"/>
+      <c r="AM74" s="58"/>
+      <c r="AN74" s="58"/>
+      <c r="AO74" s="58"/>
+      <c r="AP74" s="58"/>
+      <c r="AQ74" s="58"/>
+      <c r="AR74" s="58"/>
+      <c r="AS74" s="58"/>
+      <c r="AT74" s="58"/>
+      <c r="AU74" s="58"/>
+      <c r="AV74" s="58"/>
     </row>
     <row r="75" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y75" s="56"/>
-      <c r="AL75" s="56"/>
-      <c r="AM75" s="56"/>
-      <c r="AN75" s="56"/>
-      <c r="AO75" s="56"/>
-      <c r="AP75" s="56"/>
-      <c r="AQ75" s="56"/>
-      <c r="AR75" s="56"/>
-      <c r="AS75" s="56"/>
-      <c r="AT75" s="56"/>
-      <c r="AU75" s="56"/>
-      <c r="AV75" s="56"/>
+      <c r="Y75" s="58"/>
+      <c r="AL75" s="58"/>
+      <c r="AM75" s="58"/>
+      <c r="AN75" s="58"/>
+      <c r="AO75" s="58"/>
+      <c r="AP75" s="58"/>
+      <c r="AQ75" s="58"/>
+      <c r="AR75" s="58"/>
+      <c r="AS75" s="58"/>
+      <c r="AT75" s="58"/>
+      <c r="AU75" s="58"/>
+      <c r="AV75" s="58"/>
     </row>
     <row r="76" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y76" s="56"/>
-      <c r="AL76" s="56"/>
-      <c r="AM76" s="56"/>
-      <c r="AN76" s="56"/>
-      <c r="AO76" s="56"/>
-      <c r="AP76" s="56"/>
-      <c r="AQ76" s="56"/>
-      <c r="AR76" s="56"/>
-      <c r="AS76" s="56"/>
-      <c r="AT76" s="56"/>
-      <c r="AU76" s="56"/>
-      <c r="AV76" s="56"/>
+      <c r="Y76" s="58"/>
+      <c r="AL76" s="58"/>
+      <c r="AM76" s="58"/>
+      <c r="AN76" s="58"/>
+      <c r="AO76" s="58"/>
+      <c r="AP76" s="58"/>
+      <c r="AQ76" s="58"/>
+      <c r="AR76" s="58"/>
+      <c r="AS76" s="58"/>
+      <c r="AT76" s="58"/>
+      <c r="AU76" s="58"/>
+      <c r="AV76" s="58"/>
     </row>
     <row r="77" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y77" s="56"/>
-      <c r="AL77" s="56"/>
-      <c r="AM77" s="56"/>
-      <c r="AN77" s="56"/>
-      <c r="AO77" s="56"/>
-      <c r="AP77" s="56"/>
-      <c r="AQ77" s="56"/>
-      <c r="AR77" s="56"/>
-      <c r="AS77" s="56"/>
-      <c r="AT77" s="56"/>
-      <c r="AU77" s="56"/>
-      <c r="AV77" s="56"/>
+      <c r="Y77" s="58"/>
+      <c r="AL77" s="58"/>
+      <c r="AM77" s="58"/>
+      <c r="AN77" s="58"/>
+      <c r="AO77" s="58"/>
+      <c r="AP77" s="58"/>
+      <c r="AQ77" s="58"/>
+      <c r="AR77" s="58"/>
+      <c r="AS77" s="58"/>
+      <c r="AT77" s="58"/>
+      <c r="AU77" s="58"/>
+      <c r="AV77" s="58"/>
     </row>
     <row r="78" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y78" s="56"/>
-      <c r="AL78" s="56"/>
-      <c r="AM78" s="56"/>
-      <c r="AN78" s="56"/>
-      <c r="AO78" s="56"/>
-      <c r="AP78" s="56"/>
-      <c r="AQ78" s="56"/>
-      <c r="AR78" s="56"/>
-      <c r="AS78" s="56"/>
-      <c r="AT78" s="56"/>
-      <c r="AU78" s="56"/>
-      <c r="AV78" s="56"/>
+      <c r="Y78" s="58"/>
+      <c r="AL78" s="58"/>
+      <c r="AM78" s="58"/>
+      <c r="AN78" s="58"/>
+      <c r="AO78" s="58"/>
+      <c r="AP78" s="58"/>
+      <c r="AQ78" s="58"/>
+      <c r="AR78" s="58"/>
+      <c r="AS78" s="58"/>
+      <c r="AT78" s="58"/>
+      <c r="AU78" s="58"/>
+      <c r="AV78" s="58"/>
     </row>
     <row r="79" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y79" s="56"/>
-      <c r="AL79" s="56"/>
-      <c r="AM79" s="56"/>
-      <c r="AN79" s="56"/>
-      <c r="AO79" s="56"/>
-      <c r="AP79" s="56"/>
-      <c r="AQ79" s="56"/>
-      <c r="AR79" s="56"/>
-      <c r="AS79" s="56"/>
-      <c r="AT79" s="56"/>
-      <c r="AU79" s="56"/>
-      <c r="AV79" s="56"/>
+      <c r="Y79" s="58"/>
+      <c r="AL79" s="58"/>
+      <c r="AM79" s="58"/>
+      <c r="AN79" s="58"/>
+      <c r="AO79" s="58"/>
+      <c r="AP79" s="58"/>
+      <c r="AQ79" s="58"/>
+      <c r="AR79" s="58"/>
+      <c r="AS79" s="58"/>
+      <c r="AT79" s="58"/>
+      <c r="AU79" s="58"/>
+      <c r="AV79" s="58"/>
     </row>
     <row r="80" spans="1:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y80" s="56"/>
-      <c r="AL80" s="56"/>
-      <c r="AM80" s="56"/>
-      <c r="AN80" s="56"/>
-      <c r="AO80" s="56"/>
-      <c r="AP80" s="56"/>
-      <c r="AQ80" s="56"/>
-      <c r="AR80" s="56"/>
-      <c r="AS80" s="56"/>
-      <c r="AT80" s="56"/>
-      <c r="AU80" s="56"/>
-      <c r="AV80" s="56"/>
+      <c r="Y80" s="58"/>
+      <c r="AL80" s="58"/>
+      <c r="AM80" s="58"/>
+      <c r="AN80" s="58"/>
+      <c r="AO80" s="58"/>
+      <c r="AP80" s="58"/>
+      <c r="AQ80" s="58"/>
+      <c r="AR80" s="58"/>
+      <c r="AS80" s="58"/>
+      <c r="AT80" s="58"/>
+      <c r="AU80" s="58"/>
+      <c r="AV80" s="58"/>
     </row>
     <row r="81" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y81" s="56"/>
-      <c r="AL81" s="56"/>
-      <c r="AM81" s="56"/>
-      <c r="AN81" s="56"/>
-      <c r="AO81" s="56"/>
-      <c r="AP81" s="56"/>
-      <c r="AQ81" s="56"/>
-      <c r="AR81" s="56"/>
-      <c r="AS81" s="56"/>
-      <c r="AT81" s="56"/>
-      <c r="AU81" s="56"/>
-      <c r="AV81" s="56"/>
+      <c r="Y81" s="58"/>
+      <c r="AL81" s="58"/>
+      <c r="AM81" s="58"/>
+      <c r="AN81" s="58"/>
+      <c r="AO81" s="58"/>
+      <c r="AP81" s="58"/>
+      <c r="AQ81" s="58"/>
+      <c r="AR81" s="58"/>
+      <c r="AS81" s="58"/>
+      <c r="AT81" s="58"/>
+      <c r="AU81" s="58"/>
+      <c r="AV81" s="58"/>
     </row>
     <row r="82" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y82" s="56"/>
-      <c r="AL82" s="56"/>
-      <c r="AM82" s="56"/>
-      <c r="AN82" s="56"/>
-      <c r="AO82" s="56"/>
-      <c r="AP82" s="56"/>
-      <c r="AQ82" s="56"/>
-      <c r="AR82" s="56"/>
-      <c r="AS82" s="56"/>
-      <c r="AT82" s="56"/>
-      <c r="AU82" s="56"/>
-      <c r="AV82" s="56"/>
+      <c r="Y82" s="58"/>
+      <c r="AL82" s="58"/>
+      <c r="AM82" s="58"/>
+      <c r="AN82" s="58"/>
+      <c r="AO82" s="58"/>
+      <c r="AP82" s="58"/>
+      <c r="AQ82" s="58"/>
+      <c r="AR82" s="58"/>
+      <c r="AS82" s="58"/>
+      <c r="AT82" s="58"/>
+      <c r="AU82" s="58"/>
+      <c r="AV82" s="58"/>
     </row>
     <row r="83" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y83" s="56"/>
-      <c r="AL83" s="56"/>
-      <c r="AM83" s="56"/>
-      <c r="AN83" s="56"/>
-      <c r="AO83" s="56"/>
-      <c r="AP83" s="56"/>
-      <c r="AQ83" s="56"/>
-      <c r="AR83" s="56"/>
-      <c r="AS83" s="56"/>
-      <c r="AT83" s="56"/>
-      <c r="AU83" s="56"/>
-      <c r="AV83" s="56"/>
+      <c r="Y83" s="58"/>
+      <c r="AL83" s="58"/>
+      <c r="AM83" s="58"/>
+      <c r="AN83" s="58"/>
+      <c r="AO83" s="58"/>
+      <c r="AP83" s="58"/>
+      <c r="AQ83" s="58"/>
+      <c r="AR83" s="58"/>
+      <c r="AS83" s="58"/>
+      <c r="AT83" s="58"/>
+      <c r="AU83" s="58"/>
+      <c r="AV83" s="58"/>
     </row>
     <row r="84" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y84" s="56"/>
-      <c r="AL84" s="56"/>
-      <c r="AM84" s="56"/>
-      <c r="AN84" s="56"/>
-      <c r="AO84" s="56"/>
-      <c r="AP84" s="56"/>
-      <c r="AQ84" s="56"/>
-      <c r="AR84" s="56"/>
-      <c r="AS84" s="56"/>
-      <c r="AT84" s="56"/>
-      <c r="AU84" s="56"/>
-      <c r="AV84" s="56"/>
+      <c r="Y84" s="58"/>
+      <c r="AL84" s="58"/>
+      <c r="AM84" s="58"/>
+      <c r="AN84" s="58"/>
+      <c r="AO84" s="58"/>
+      <c r="AP84" s="58"/>
+      <c r="AQ84" s="58"/>
+      <c r="AR84" s="58"/>
+      <c r="AS84" s="58"/>
+      <c r="AT84" s="58"/>
+      <c r="AU84" s="58"/>
+      <c r="AV84" s="58"/>
     </row>
     <row r="85" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y85" s="56"/>
-      <c r="AL85" s="56"/>
-      <c r="AM85" s="56"/>
-      <c r="AN85" s="56"/>
-      <c r="AO85" s="56"/>
-      <c r="AP85" s="56"/>
-      <c r="AQ85" s="56"/>
-      <c r="AR85" s="56"/>
-      <c r="AS85" s="56"/>
-      <c r="AT85" s="56"/>
-      <c r="AU85" s="56"/>
-      <c r="AV85" s="56"/>
+      <c r="Y85" s="58"/>
+      <c r="AL85" s="58"/>
+      <c r="AM85" s="58"/>
+      <c r="AN85" s="58"/>
+      <c r="AO85" s="58"/>
+      <c r="AP85" s="58"/>
+      <c r="AQ85" s="58"/>
+      <c r="AR85" s="58"/>
+      <c r="AS85" s="58"/>
+      <c r="AT85" s="58"/>
+      <c r="AU85" s="58"/>
+      <c r="AV85" s="58"/>
     </row>
     <row r="86" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y86" s="56"/>
-      <c r="AL86" s="56"/>
-      <c r="AM86" s="56"/>
-      <c r="AN86" s="56"/>
-      <c r="AO86" s="56"/>
-      <c r="AP86" s="56"/>
-      <c r="AQ86" s="56"/>
-      <c r="AR86" s="56"/>
-      <c r="AS86" s="56"/>
-      <c r="AT86" s="56"/>
-      <c r="AU86" s="56"/>
-      <c r="AV86" s="56"/>
+      <c r="Y86" s="58"/>
+      <c r="AL86" s="58"/>
+      <c r="AM86" s="58"/>
+      <c r="AN86" s="58"/>
+      <c r="AO86" s="58"/>
+      <c r="AP86" s="58"/>
+      <c r="AQ86" s="58"/>
+      <c r="AR86" s="58"/>
+      <c r="AS86" s="58"/>
+      <c r="AT86" s="58"/>
+      <c r="AU86" s="58"/>
+      <c r="AV86" s="58"/>
     </row>
     <row r="87" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y87" s="56"/>
-      <c r="AL87" s="56"/>
-      <c r="AM87" s="56"/>
-      <c r="AN87" s="56"/>
-      <c r="AO87" s="56"/>
-      <c r="AP87" s="56"/>
-      <c r="AQ87" s="56"/>
-      <c r="AR87" s="56"/>
-      <c r="AS87" s="56"/>
-      <c r="AT87" s="56"/>
-      <c r="AU87" s="56"/>
-      <c r="AV87" s="56"/>
+      <c r="Y87" s="58"/>
+      <c r="AL87" s="58"/>
+      <c r="AM87" s="58"/>
+      <c r="AN87" s="58"/>
+      <c r="AO87" s="58"/>
+      <c r="AP87" s="58"/>
+      <c r="AQ87" s="58"/>
+      <c r="AR87" s="58"/>
+      <c r="AS87" s="58"/>
+      <c r="AT87" s="58"/>
+      <c r="AU87" s="58"/>
+      <c r="AV87" s="58"/>
     </row>
     <row r="88" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y88" s="56"/>
-      <c r="AL88" s="56"/>
-      <c r="AM88" s="56"/>
-      <c r="AN88" s="56"/>
-      <c r="AO88" s="56"/>
-      <c r="AP88" s="56"/>
-      <c r="AQ88" s="56"/>
-      <c r="AR88" s="56"/>
-      <c r="AS88" s="56"/>
-      <c r="AT88" s="56"/>
-      <c r="AU88" s="56"/>
-      <c r="AV88" s="56"/>
+      <c r="Y88" s="58"/>
+      <c r="AL88" s="58"/>
+      <c r="AM88" s="58"/>
+      <c r="AN88" s="58"/>
+      <c r="AO88" s="58"/>
+      <c r="AP88" s="58"/>
+      <c r="AQ88" s="58"/>
+      <c r="AR88" s="58"/>
+      <c r="AS88" s="58"/>
+      <c r="AT88" s="58"/>
+      <c r="AU88" s="58"/>
+      <c r="AV88" s="58"/>
     </row>
     <row r="89" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y89" s="56"/>
-      <c r="AL89" s="56"/>
-      <c r="AM89" s="56"/>
-      <c r="AN89" s="56"/>
-      <c r="AO89" s="56"/>
-      <c r="AP89" s="56"/>
-      <c r="AQ89" s="56"/>
-      <c r="AR89" s="56"/>
-      <c r="AS89" s="56"/>
-      <c r="AT89" s="56"/>
-      <c r="AU89" s="56"/>
-      <c r="AV89" s="56"/>
+      <c r="Y89" s="58"/>
+      <c r="AL89" s="58"/>
+      <c r="AM89" s="58"/>
+      <c r="AN89" s="58"/>
+      <c r="AO89" s="58"/>
+      <c r="AP89" s="58"/>
+      <c r="AQ89" s="58"/>
+      <c r="AR89" s="58"/>
+      <c r="AS89" s="58"/>
+      <c r="AT89" s="58"/>
+      <c r="AU89" s="58"/>
+      <c r="AV89" s="58"/>
     </row>
     <row r="90" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y90" s="56"/>
-      <c r="AL90" s="56"/>
-      <c r="AM90" s="56"/>
-      <c r="AN90" s="56"/>
-      <c r="AO90" s="56"/>
-      <c r="AP90" s="56"/>
-      <c r="AQ90" s="56"/>
-      <c r="AR90" s="56"/>
-      <c r="AS90" s="56"/>
-      <c r="AT90" s="56"/>
-      <c r="AU90" s="56"/>
-      <c r="AV90" s="56"/>
+      <c r="Y90" s="58"/>
+      <c r="AL90" s="58"/>
+      <c r="AM90" s="58"/>
+      <c r="AN90" s="58"/>
+      <c r="AO90" s="58"/>
+      <c r="AP90" s="58"/>
+      <c r="AQ90" s="58"/>
+      <c r="AR90" s="58"/>
+      <c r="AS90" s="58"/>
+      <c r="AT90" s="58"/>
+      <c r="AU90" s="58"/>
+      <c r="AV90" s="58"/>
     </row>
     <row r="91" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y91" s="56"/>
-      <c r="AL91" s="56"/>
-      <c r="AM91" s="56"/>
-      <c r="AN91" s="56"/>
-      <c r="AO91" s="56"/>
-      <c r="AP91" s="56"/>
-      <c r="AQ91" s="56"/>
-      <c r="AR91" s="56"/>
-      <c r="AS91" s="56"/>
-      <c r="AT91" s="56"/>
-      <c r="AU91" s="56"/>
-      <c r="AV91" s="56"/>
+      <c r="Y91" s="58"/>
+      <c r="AL91" s="58"/>
+      <c r="AM91" s="58"/>
+      <c r="AN91" s="58"/>
+      <c r="AO91" s="58"/>
+      <c r="AP91" s="58"/>
+      <c r="AQ91" s="58"/>
+      <c r="AR91" s="58"/>
+      <c r="AS91" s="58"/>
+      <c r="AT91" s="58"/>
+      <c r="AU91" s="58"/>
+      <c r="AV91" s="58"/>
     </row>
     <row r="92" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y92" s="56"/>
-      <c r="AL92" s="56"/>
-      <c r="AM92" s="56"/>
-      <c r="AN92" s="56"/>
-      <c r="AO92" s="56"/>
-      <c r="AP92" s="56"/>
-      <c r="AQ92" s="56"/>
-      <c r="AR92" s="56"/>
-      <c r="AS92" s="56"/>
-      <c r="AT92" s="56"/>
-      <c r="AU92" s="56"/>
-      <c r="AV92" s="56"/>
+      <c r="Y92" s="58"/>
+      <c r="AL92" s="58"/>
+      <c r="AM92" s="58"/>
+      <c r="AN92" s="58"/>
+      <c r="AO92" s="58"/>
+      <c r="AP92" s="58"/>
+      <c r="AQ92" s="58"/>
+      <c r="AR92" s="58"/>
+      <c r="AS92" s="58"/>
+      <c r="AT92" s="58"/>
+      <c r="AU92" s="58"/>
+      <c r="AV92" s="58"/>
     </row>
     <row r="93" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y93" s="56"/>
-      <c r="AL93" s="56"/>
-      <c r="AM93" s="56"/>
-      <c r="AN93" s="56"/>
-      <c r="AO93" s="56"/>
-      <c r="AP93" s="56"/>
-      <c r="AQ93" s="56"/>
-      <c r="AR93" s="56"/>
-      <c r="AS93" s="56"/>
-      <c r="AT93" s="56"/>
-      <c r="AU93" s="56"/>
-      <c r="AV93" s="56"/>
+      <c r="Y93" s="58"/>
+      <c r="AL93" s="58"/>
+      <c r="AM93" s="58"/>
+      <c r="AN93" s="58"/>
+      <c r="AO93" s="58"/>
+      <c r="AP93" s="58"/>
+      <c r="AQ93" s="58"/>
+      <c r="AR93" s="58"/>
+      <c r="AS93" s="58"/>
+      <c r="AT93" s="58"/>
+      <c r="AU93" s="58"/>
+      <c r="AV93" s="58"/>
     </row>
     <row r="94" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y94" s="56"/>
-      <c r="AL94" s="56"/>
-      <c r="AM94" s="56"/>
-      <c r="AN94" s="56"/>
-      <c r="AO94" s="56"/>
-      <c r="AP94" s="56"/>
-      <c r="AQ94" s="56"/>
-      <c r="AR94" s="56"/>
-      <c r="AS94" s="56"/>
-      <c r="AT94" s="56"/>
-      <c r="AU94" s="56"/>
-      <c r="AV94" s="56"/>
+      <c r="Y94" s="58"/>
+      <c r="AL94" s="58"/>
+      <c r="AM94" s="58"/>
+      <c r="AN94" s="58"/>
+      <c r="AO94" s="58"/>
+      <c r="AP94" s="58"/>
+      <c r="AQ94" s="58"/>
+      <c r="AR94" s="58"/>
+      <c r="AS94" s="58"/>
+      <c r="AT94" s="58"/>
+      <c r="AU94" s="58"/>
+      <c r="AV94" s="58"/>
     </row>
     <row r="95" spans="25:48" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y95" s="56"/>
-      <c r="AL95" s="56"/>
-      <c r="AM95" s="56"/>
-      <c r="AN95" s="56"/>
-      <c r="AO95" s="56"/>
-      <c r="AP95" s="56"/>
-      <c r="AQ95" s="56"/>
-      <c r="AR95" s="56"/>
-      <c r="AS95" s="56"/>
-      <c r="AT95" s="56"/>
-      <c r="AU95" s="56"/>
-      <c r="AV95" s="56"/>
+      <c r="Y95" s="58"/>
+      <c r="AL95" s="58"/>
+      <c r="AM95" s="58"/>
+      <c r="AN95" s="58"/>
+      <c r="AO95" s="58"/>
+      <c r="AP95" s="58"/>
+      <c r="AQ95" s="58"/>
+      <c r="AR95" s="58"/>
+      <c r="AS95" s="58"/>
+      <c r="AT95" s="58"/>
+      <c r="AU95" s="58"/>
+      <c r="AV95" s="58"/>
     </row>
     <row r="98" spans="15:40" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O98" s="56"/>
-      <c r="P98" s="56"/>
+      <c r="O98" s="58"/>
+      <c r="P98" s="58"/>
     </row>
     <row r="99" spans="15:40" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL99" s="56"/>
-      <c r="AM99" s="56"/>
-      <c r="AN99" s="56"/>
+      <c r="AL99" s="58"/>
+      <c r="AM99" s="58"/>
+      <c r="AN99" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6099,21 +6085,21 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
       <selection activeCell="G8" sqref="G8:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="32.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="60" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.5" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26" style="60" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" style="60" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" style="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -6248,61 +6234,61 @@
       <c r="J7" s="97"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71">
+      <c r="A8" s="56">
         <v>1021</v>
       </c>
-      <c r="B8" s="71" t="s">
+      <c r="B8" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="57" t="s">
         <v>241</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="56">
         <v>37.1</v>
       </c>
-      <c r="J8" s="71">
+      <c r="J8" s="56">
         <f t="shared" ref="J8:J28" si="0">AVERAGE(D8:H8)</f>
         <v>37.1</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71">
+      <c r="A9" s="56">
         <v>1225</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="G9" s="71">
+      <c r="G9" s="56">
         <v>44.4</v>
       </c>
-      <c r="H9" s="71">
+      <c r="H9" s="56">
         <v>43.8</v>
       </c>
-      <c r="J9" s="71">
+      <c r="J9" s="56">
         <f t="shared" si="0"/>
         <v>44.099999999999994</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="71">
+      <c r="A10" s="56">
         <v>1227</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="57" t="s">
         <v>243</v>
       </c>
-      <c r="G10" s="71">
+      <c r="G10" s="56">
         <v>62.2</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="56">
         <v>66.7</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10" s="56">
         <f t="shared" si="0"/>
         <v>64.45</v>
       </c>
@@ -6320,13 +6306,13 @@
       <c r="F11" s="45">
         <v>0</v>
       </c>
-      <c r="G11" s="71">
+      <c r="G11" s="56">
         <v>21.5</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="56">
         <v>62.5</v>
       </c>
-      <c r="J11" s="71">
+      <c r="J11" s="56">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -6344,55 +6330,55 @@
       <c r="F12" s="45">
         <v>0</v>
       </c>
-      <c r="G12" s="71">
+      <c r="G12" s="56">
         <v>83.5</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="56">
         <v>100</v>
       </c>
-      <c r="J12" s="71">
+      <c r="J12" s="56">
         <f t="shared" si="0"/>
         <v>61.166666666666664</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="71">
+      <c r="A13" s="56">
         <v>1240</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="72" t="s">
+      <c r="C13" s="57" t="s">
         <v>246</v>
       </c>
-      <c r="G13" s="71">
+      <c r="G13" s="56">
         <v>38.1</v>
       </c>
-      <c r="H13" s="71">
+      <c r="H13" s="56">
         <v>43.8</v>
       </c>
-      <c r="J13" s="71">
+      <c r="J13" s="56">
         <f t="shared" si="0"/>
         <v>40.950000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71">
+      <c r="A14" s="56">
         <v>1248</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="G14" s="71">
+      <c r="G14" s="56">
         <v>40.200000000000003</v>
       </c>
-      <c r="H14" s="71">
+      <c r="H14" s="56">
         <v>40.700000000000003</v>
       </c>
-      <c r="J14" s="71">
+      <c r="J14" s="56">
         <f t="shared" si="0"/>
         <v>40.450000000000003</v>
       </c>
@@ -6410,73 +6396,73 @@
       <c r="F15" s="45">
         <v>0</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="56">
         <v>67.7</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="56">
         <v>74.2</v>
       </c>
-      <c r="J15" s="71">
+      <c r="J15" s="56">
         <f t="shared" si="0"/>
         <v>47.300000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71">
+      <c r="A16" s="56">
         <v>1402</v>
       </c>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="G16" s="71">
+      <c r="G16" s="56">
         <v>56.5</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="56">
         <v>48.2</v>
       </c>
-      <c r="J16" s="71">
+      <c r="J16" s="56">
         <f t="shared" si="0"/>
         <v>52.35</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71">
+      <c r="A17" s="56">
         <v>1412</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="H17" s="71">
+      <c r="H17" s="56">
         <v>79.2</v>
       </c>
-      <c r="J17" s="71">
+      <c r="J17" s="56">
         <f t="shared" si="0"/>
         <v>79.2</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="71">
+      <c r="A18" s="56">
         <v>1512</v>
       </c>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="G18" s="71">
+      <c r="G18" s="56">
         <v>50</v>
       </c>
-      <c r="H18" s="71">
+      <c r="H18" s="56">
         <v>50</v>
       </c>
-      <c r="J18" s="71">
+      <c r="J18" s="56">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
@@ -6494,18 +6480,18 @@
       <c r="F19" s="45">
         <v>6.9</v>
       </c>
-      <c r="G19" s="71">
+      <c r="G19" s="56">
         <v>73.2</v>
       </c>
-      <c r="H19" s="71">
+      <c r="H19" s="56">
         <v>58.3</v>
       </c>
-      <c r="J19" s="71">
+      <c r="J19" s="56">
         <f t="shared" si="0"/>
         <v>46.133333333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="45">
         <v>1678</v>
       </c>
@@ -6518,39 +6504,39 @@
       <c r="F20" s="45">
         <v>0</v>
       </c>
-      <c r="G20" s="71">
+      <c r="G20" s="56">
         <v>43.8</v>
       </c>
-      <c r="H20" s="71">
+      <c r="H20" s="56">
         <v>49.3</v>
       </c>
-      <c r="J20" s="71">
+      <c r="J20" s="56">
         <f t="shared" si="0"/>
         <v>31.033333333333331</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="A21" s="71">
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="56">
         <v>1705</v>
       </c>
-      <c r="B21" s="71" t="s">
+      <c r="B21" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="57" t="s">
         <v>254</v>
       </c>
-      <c r="G21" s="71">
+      <c r="G21" s="56">
         <v>77.8</v>
       </c>
-      <c r="H21" s="71">
+      <c r="H21" s="56">
         <v>64.2</v>
       </c>
-      <c r="J21" s="71">
+      <c r="J21" s="56">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="45">
         <v>1711</v>
       </c>
@@ -6563,18 +6549,18 @@
       <c r="F22" s="45">
         <v>0</v>
       </c>
-      <c r="G22" s="71">
+      <c r="G22" s="56">
         <v>39.9</v>
       </c>
-      <c r="H22" s="71">
+      <c r="H22" s="56">
         <v>23.8</v>
       </c>
-      <c r="J22" s="71">
+      <c r="J22" s="56">
         <f t="shared" si="0"/>
         <v>21.233333333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45">
         <v>50123</v>
       </c>
@@ -6587,18 +6573,18 @@
       <c r="F23" s="45">
         <v>0</v>
       </c>
-      <c r="G23" s="71">
+      <c r="G23" s="56">
         <v>59.9</v>
       </c>
-      <c r="H23" s="71">
+      <c r="H23" s="56">
         <v>78.099999999999994</v>
       </c>
-      <c r="J23" s="71">
+      <c r="J23" s="56">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="45">
         <v>50195</v>
       </c>
@@ -6611,18 +6597,18 @@
       <c r="F24" s="45">
         <v>0</v>
       </c>
-      <c r="G24" s="71">
+      <c r="G24" s="56">
         <v>68.3</v>
       </c>
-      <c r="H24" s="71">
+      <c r="H24" s="56">
         <v>59.7</v>
       </c>
-      <c r="J24" s="71">
+      <c r="J24" s="56">
         <f t="shared" si="0"/>
         <v>42.666666666666664</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="45">
         <v>50199</v>
       </c>
@@ -6635,18 +6621,18 @@
       <c r="F25" s="45">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G25" s="71">
+      <c r="G25" s="56">
         <v>98.3</v>
       </c>
-      <c r="H25" s="71">
+      <c r="H25" s="56">
         <v>58.3</v>
       </c>
-      <c r="J25" s="71">
+      <c r="J25" s="56">
         <f t="shared" si="0"/>
         <v>55.29999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="45">
         <v>50234</v>
       </c>
@@ -6659,18 +6645,18 @@
       <c r="F26" s="45">
         <v>0</v>
       </c>
-      <c r="G26" s="71">
-        <v>0</v>
-      </c>
-      <c r="H26" s="71">
-        <v>0</v>
-      </c>
-      <c r="J26" s="71">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+      <c r="G26" s="56">
+        <v>0</v>
+      </c>
+      <c r="H26" s="56">
+        <v>0</v>
+      </c>
+      <c r="J26" s="56">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="45">
         <v>50265</v>
       </c>
@@ -6683,18 +6669,18 @@
       <c r="F27" s="45">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G27" s="71">
+      <c r="G27" s="56">
         <v>27.3</v>
       </c>
-      <c r="H27" s="71">
+      <c r="H27" s="56">
         <v>27.5</v>
       </c>
-      <c r="J27" s="71">
+      <c r="J27" s="56">
         <f t="shared" si="0"/>
         <v>21.366666666666664</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="45">
         <v>50294</v>
       </c>
@@ -6707,13 +6693,13 @@
       <c r="F28" s="45">
         <v>0</v>
       </c>
-      <c r="G28" s="71">
+      <c r="G28" s="56">
         <v>39.1</v>
       </c>
-      <c r="H28" s="71">
+      <c r="H28" s="56">
         <v>41.7</v>
       </c>
-      <c r="J28" s="71">
+      <c r="J28" s="56">
         <f t="shared" si="0"/>
         <v>26.933333333333337</v>
       </c>
@@ -6729,18 +6715,6 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="J5:J7"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6758,11 +6732,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -7074,11 +7048,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="70" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="70" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8035,11 +8009,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="80" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="80" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -8798,11 +8772,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="70" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="70" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -9579,11 +9553,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="72.5" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="72.5" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -10639,11 +10613,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="82.5" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="82.5" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -11834,11 +11808,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -12024,17 +11998,17 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="50" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="50" workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.5" style="58" customWidth="1"/>
-    <col min="3" max="3" width="75" style="58" customWidth="1"/>
-    <col min="4" max="8" width="21.5" style="58" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="21.5" style="58" customWidth="1"/>
+    <col min="1" max="2" width="21.5" style="60" customWidth="1"/>
+    <col min="3" max="3" width="75" style="60" customWidth="1"/>
+    <col min="4" max="8" width="21.5" style="60" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="60" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -12187,13 +12161,13 @@
       <c r="F8" s="45">
         <v>19.3</v>
       </c>
-      <c r="G8" s="71">
+      <c r="G8" s="56">
         <v>20.2</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="56">
         <v>24.1</v>
       </c>
-      <c r="J8" s="71">
+      <c r="J8" s="56">
         <f t="shared" ref="J8:J52" si="0">AVERAGE(D8:H8)</f>
         <v>21.619999999999997</v>
       </c>
@@ -12217,13 +12191,13 @@
       <c r="F9" s="45">
         <v>35</v>
       </c>
-      <c r="G9" s="71">
+      <c r="G9" s="56">
         <v>40.4</v>
       </c>
-      <c r="H9" s="71">
+      <c r="H9" s="56">
         <v>55.1</v>
       </c>
-      <c r="J9" s="71">
+      <c r="J9" s="56">
         <f t="shared" si="0"/>
         <v>42.44</v>
       </c>
@@ -12247,13 +12221,13 @@
       <c r="F10" s="45">
         <v>23.2</v>
       </c>
-      <c r="G10" s="71">
+      <c r="G10" s="56">
         <v>33.4</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="56">
         <v>26.5</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10" s="56">
         <f t="shared" si="0"/>
         <v>29.619999999999997</v>
       </c>
@@ -12277,13 +12251,13 @@
       <c r="F11" s="45">
         <v>21.9</v>
       </c>
-      <c r="G11" s="71">
+      <c r="G11" s="56">
         <v>21.8</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="56">
         <v>31.2</v>
       </c>
-      <c r="J11" s="71">
+      <c r="J11" s="56">
         <f t="shared" si="0"/>
         <v>23.72</v>
       </c>
@@ -12307,13 +12281,13 @@
       <c r="F12" s="45">
         <v>28.2</v>
       </c>
-      <c r="G12" s="71">
-        <v>0</v>
-      </c>
-      <c r="H12" s="71">
-        <v>0</v>
-      </c>
-      <c r="J12" s="71">
+      <c r="G12" s="56">
+        <v>0</v>
+      </c>
+      <c r="H12" s="56">
+        <v>0</v>
+      </c>
+      <c r="J12" s="56">
         <f t="shared" si="0"/>
         <v>15.98</v>
       </c>
@@ -12337,13 +12311,13 @@
       <c r="F13" s="45">
         <v>24.1</v>
       </c>
-      <c r="G13" s="71">
+      <c r="G13" s="56">
         <v>28.8</v>
       </c>
-      <c r="H13" s="71">
+      <c r="H13" s="56">
         <v>117.3</v>
       </c>
-      <c r="J13" s="71">
+      <c r="J13" s="56">
         <f t="shared" si="0"/>
         <v>46.279999999999994</v>
       </c>
@@ -12361,13 +12335,13 @@
       <c r="F14" s="45">
         <v>26.9</v>
       </c>
-      <c r="G14" s="71">
+      <c r="G14" s="56">
         <v>33.700000000000003</v>
       </c>
-      <c r="H14" s="71">
+      <c r="H14" s="56">
         <v>29</v>
       </c>
-      <c r="J14" s="71">
+      <c r="J14" s="56">
         <f t="shared" si="0"/>
         <v>29.866666666666664</v>
       </c>
@@ -12391,13 +12365,13 @@
       <c r="F15" s="45">
         <v>21.9</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="56">
         <v>23.1</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="56">
         <v>27.4</v>
       </c>
-      <c r="J15" s="71">
+      <c r="J15" s="56">
         <f t="shared" si="0"/>
         <v>28.4</v>
       </c>
@@ -12421,13 +12395,13 @@
       <c r="F16" s="45">
         <v>35.9</v>
       </c>
-      <c r="G16" s="71">
+      <c r="G16" s="56">
         <v>41.2</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="56">
         <v>43.3</v>
       </c>
-      <c r="J16" s="71">
+      <c r="J16" s="56">
         <f t="shared" si="0"/>
         <v>35.260000000000005</v>
       </c>
@@ -12451,13 +12425,13 @@
       <c r="F17" s="45">
         <v>10.4</v>
       </c>
-      <c r="G17" s="71">
+      <c r="G17" s="56">
         <v>12.4</v>
       </c>
-      <c r="H17" s="71">
+      <c r="H17" s="56">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J17" s="71">
+      <c r="J17" s="56">
         <f t="shared" si="0"/>
         <v>10.52</v>
       </c>
@@ -12481,13 +12455,13 @@
       <c r="F18" s="45">
         <v>10.9</v>
       </c>
-      <c r="G18" s="71">
+      <c r="G18" s="56">
         <v>11.4</v>
       </c>
-      <c r="H18" s="71">
+      <c r="H18" s="56">
         <v>15.3</v>
       </c>
-      <c r="J18" s="71">
+      <c r="J18" s="56">
         <f t="shared" si="0"/>
         <v>15.779999999999998</v>
       </c>
@@ -12511,13 +12485,13 @@
       <c r="F19" s="45">
         <v>10.199999999999999</v>
       </c>
-      <c r="G19" s="71">
+      <c r="G19" s="56">
         <v>23.5</v>
       </c>
-      <c r="H19" s="71">
+      <c r="H19" s="56">
         <v>31.9</v>
       </c>
-      <c r="J19" s="71">
+      <c r="J19" s="56">
         <f t="shared" si="0"/>
         <v>20.68</v>
       </c>
@@ -12541,13 +12515,13 @@
       <c r="F20" s="45">
         <v>11.1</v>
       </c>
-      <c r="G20" s="71">
+      <c r="G20" s="56">
         <v>16.3</v>
       </c>
-      <c r="H20" s="71">
+      <c r="H20" s="56">
         <v>12.3</v>
       </c>
-      <c r="J20" s="71">
+      <c r="J20" s="56">
         <f t="shared" si="0"/>
         <v>12.3</v>
       </c>
@@ -12571,13 +12545,13 @@
       <c r="F21" s="45">
         <v>21.9</v>
       </c>
-      <c r="G21" s="71">
+      <c r="G21" s="56">
         <v>21.9</v>
       </c>
-      <c r="H21" s="71">
+      <c r="H21" s="56">
         <v>29.5</v>
       </c>
-      <c r="J21" s="71">
+      <c r="J21" s="56">
         <f t="shared" si="0"/>
         <v>24.68</v>
       </c>
@@ -12601,13 +12575,13 @@
       <c r="F22" s="45">
         <v>62.1</v>
       </c>
-      <c r="G22" s="71">
+      <c r="G22" s="56">
         <v>56</v>
       </c>
-      <c r="H22" s="71">
+      <c r="H22" s="56">
         <v>76.599999999999994</v>
       </c>
-      <c r="J22" s="71">
+      <c r="J22" s="56">
         <f t="shared" si="0"/>
         <v>59.259999999999991</v>
       </c>
@@ -12631,13 +12605,13 @@
       <c r="F23" s="45">
         <v>32.1</v>
       </c>
-      <c r="G23" s="71">
+      <c r="G23" s="56">
         <v>28.9</v>
       </c>
-      <c r="H23" s="71">
+      <c r="H23" s="56">
         <v>38.5</v>
       </c>
-      <c r="J23" s="71">
+      <c r="J23" s="56">
         <f t="shared" si="0"/>
         <v>32.58</v>
       </c>
@@ -12661,13 +12635,13 @@
       <c r="F24" s="45">
         <v>7</v>
       </c>
-      <c r="G24" s="71">
+      <c r="G24" s="56">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H24" s="71">
+      <c r="H24" s="56">
         <v>3.9</v>
       </c>
-      <c r="J24" s="71">
+      <c r="J24" s="56">
         <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
@@ -12691,13 +12665,13 @@
       <c r="F25" s="45">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G25" s="71">
+      <c r="G25" s="56">
         <v>11.1</v>
       </c>
-      <c r="H25" s="71">
+      <c r="H25" s="56">
         <v>12.6</v>
       </c>
-      <c r="J25" s="71">
+      <c r="J25" s="56">
         <f t="shared" si="0"/>
         <v>10.28</v>
       </c>
@@ -12721,13 +12695,13 @@
       <c r="F26" s="45">
         <v>13.1</v>
       </c>
-      <c r="G26" s="71">
+      <c r="G26" s="56">
         <v>16.3</v>
       </c>
-      <c r="H26" s="71">
+      <c r="H26" s="56">
         <v>12.3</v>
       </c>
-      <c r="J26" s="71">
+      <c r="J26" s="56">
         <f t="shared" si="0"/>
         <v>13.780000000000001</v>
       </c>
@@ -12751,13 +12725,13 @@
       <c r="F27" s="45">
         <v>11.2</v>
       </c>
-      <c r="G27" s="71">
+      <c r="G27" s="56">
         <v>6.8</v>
       </c>
-      <c r="H27" s="71">
+      <c r="H27" s="56">
         <v>3.1</v>
       </c>
-      <c r="J27" s="71">
+      <c r="J27" s="56">
         <f t="shared" si="0"/>
         <v>9.16</v>
       </c>
@@ -12781,13 +12755,13 @@
       <c r="F28" s="45">
         <v>15.2</v>
       </c>
-      <c r="G28" s="71">
+      <c r="G28" s="56">
         <v>27.1</v>
       </c>
-      <c r="H28" s="71">
+      <c r="H28" s="56">
         <v>15.2</v>
       </c>
-      <c r="J28" s="71">
+      <c r="J28" s="56">
         <f t="shared" si="0"/>
         <v>24.780000000000005</v>
       </c>
@@ -12811,13 +12785,13 @@
       <c r="F29" s="45">
         <v>7.3</v>
       </c>
-      <c r="G29" s="71">
+      <c r="G29" s="56">
         <v>7.3</v>
       </c>
-      <c r="H29" s="71">
+      <c r="H29" s="56">
         <v>7</v>
       </c>
-      <c r="J29" s="71">
+      <c r="J29" s="56">
         <f t="shared" si="0"/>
         <v>6.6599999999999993</v>
       </c>
@@ -12841,13 +12815,13 @@
       <c r="F30" s="45">
         <v>27.5</v>
       </c>
-      <c r="G30" s="71">
+      <c r="G30" s="56">
         <v>32.1</v>
       </c>
-      <c r="H30" s="71">
+      <c r="H30" s="56">
         <v>43.8</v>
       </c>
-      <c r="J30" s="71">
+      <c r="J30" s="56">
         <f t="shared" si="0"/>
         <v>31.620000000000005</v>
       </c>
@@ -12865,13 +12839,13 @@
       <c r="F31" s="45">
         <v>49.6</v>
       </c>
-      <c r="G31" s="71">
+      <c r="G31" s="56">
         <v>54.4</v>
       </c>
-      <c r="H31" s="71">
+      <c r="H31" s="56">
         <v>69.599999999999994</v>
       </c>
-      <c r="J31" s="71">
+      <c r="J31" s="56">
         <f t="shared" si="0"/>
         <v>57.866666666666667</v>
       </c>
@@ -12895,13 +12869,13 @@
       <c r="F32" s="45">
         <v>0</v>
       </c>
-      <c r="G32" s="71">
+      <c r="G32" s="56">
         <v>30.3</v>
       </c>
-      <c r="H32" s="71">
-        <v>0</v>
-      </c>
-      <c r="J32" s="71">
+      <c r="H32" s="56">
+        <v>0</v>
+      </c>
+      <c r="J32" s="56">
         <f t="shared" si="0"/>
         <v>20.2</v>
       </c>
@@ -12925,13 +12899,13 @@
       <c r="F33" s="45">
         <v>21.7</v>
       </c>
-      <c r="G33" s="71">
+      <c r="G33" s="56">
         <v>29.2</v>
       </c>
-      <c r="H33" s="71">
+      <c r="H33" s="56">
         <v>41.2</v>
       </c>
-      <c r="J33" s="71">
+      <c r="J33" s="56">
         <f t="shared" si="0"/>
         <v>30.620000000000005</v>
       </c>
@@ -12955,13 +12929,13 @@
       <c r="F34" s="45">
         <v>25.3</v>
       </c>
-      <c r="G34" s="71">
+      <c r="G34" s="56">
         <v>30.3</v>
       </c>
-      <c r="H34" s="71">
+      <c r="H34" s="56">
         <v>22.8</v>
       </c>
-      <c r="J34" s="71">
+      <c r="J34" s="56">
         <f t="shared" si="0"/>
         <v>26.04</v>
       </c>
@@ -12982,13 +12956,13 @@
       <c r="F35" s="45">
         <v>20.6</v>
       </c>
-      <c r="G35" s="71">
+      <c r="G35" s="56">
         <v>30.9</v>
       </c>
-      <c r="H35" s="71">
+      <c r="H35" s="56">
         <v>23.2</v>
       </c>
-      <c r="J35" s="71">
+      <c r="J35" s="56">
         <f t="shared" si="0"/>
         <v>23.824999999999999</v>
       </c>
@@ -13012,13 +12986,13 @@
       <c r="F36" s="45">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G36" s="71">
+      <c r="G36" s="56">
         <v>10.6</v>
       </c>
-      <c r="H36" s="71">
-        <v>0</v>
-      </c>
-      <c r="J36" s="71">
+      <c r="H36" s="56">
+        <v>0</v>
+      </c>
+      <c r="J36" s="56">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -13042,13 +13016,13 @@
       <c r="F37" s="45">
         <v>14.4</v>
       </c>
-      <c r="G37" s="71">
+      <c r="G37" s="56">
         <v>18.100000000000001</v>
       </c>
-      <c r="H37" s="71">
+      <c r="H37" s="56">
         <v>6.4</v>
       </c>
-      <c r="J37" s="71">
+      <c r="J37" s="56">
         <f t="shared" si="0"/>
         <v>11.42</v>
       </c>
@@ -13072,13 +13046,13 @@
       <c r="F38" s="45">
         <v>21.1</v>
       </c>
-      <c r="G38" s="71">
+      <c r="G38" s="56">
         <v>25.9</v>
       </c>
-      <c r="H38" s="71">
+      <c r="H38" s="56">
         <v>14.6</v>
       </c>
-      <c r="J38" s="71">
+      <c r="J38" s="56">
         <f t="shared" si="0"/>
         <v>16.2</v>
       </c>
@@ -13102,13 +13076,13 @@
       <c r="F39" s="45">
         <v>47.3</v>
       </c>
-      <c r="G39" s="71">
+      <c r="G39" s="56">
         <v>51</v>
       </c>
-      <c r="H39" s="71">
+      <c r="H39" s="56">
         <v>35.9</v>
       </c>
-      <c r="J39" s="71">
+      <c r="J39" s="56">
         <f t="shared" si="0"/>
         <v>44.8</v>
       </c>
@@ -13132,13 +13106,13 @@
       <c r="F40" s="45">
         <v>21.8</v>
       </c>
-      <c r="G40" s="71">
+      <c r="G40" s="56">
         <v>21.3</v>
       </c>
-      <c r="H40" s="71">
+      <c r="H40" s="56">
         <v>32.700000000000003</v>
       </c>
-      <c r="J40" s="71">
+      <c r="J40" s="56">
         <f t="shared" si="0"/>
         <v>26.76</v>
       </c>
@@ -13162,13 +13136,13 @@
       <c r="F41" s="45">
         <v>19.399999999999999</v>
       </c>
-      <c r="G41" s="71">
+      <c r="G41" s="56">
         <v>19.399999999999999</v>
       </c>
-      <c r="H41" s="71">
+      <c r="H41" s="56">
         <v>14.6</v>
       </c>
-      <c r="J41" s="71">
+      <c r="J41" s="56">
         <f t="shared" si="0"/>
         <v>22.339999999999996</v>
       </c>
@@ -13192,13 +13166,13 @@
       <c r="F42" s="45">
         <v>28.5</v>
       </c>
-      <c r="G42" s="71">
+      <c r="G42" s="56">
         <v>28.5</v>
       </c>
-      <c r="H42" s="71">
+      <c r="H42" s="56">
         <v>25.7</v>
       </c>
-      <c r="J42" s="71">
+      <c r="J42" s="56">
         <f t="shared" si="0"/>
         <v>27.939999999999998</v>
       </c>
@@ -13222,13 +13196,13 @@
       <c r="F43" s="45">
         <v>15.6</v>
       </c>
-      <c r="G43" s="71">
+      <c r="G43" s="56">
         <v>9</v>
       </c>
-      <c r="H43" s="71">
+      <c r="H43" s="56">
         <v>12</v>
       </c>
-      <c r="J43" s="71">
+      <c r="J43" s="56">
         <f t="shared" si="0"/>
         <v>16.380000000000003</v>
       </c>
@@ -13252,13 +13226,13 @@
       <c r="F44" s="45">
         <v>4</v>
       </c>
-      <c r="G44" s="71">
+      <c r="G44" s="56">
         <v>3.8</v>
       </c>
-      <c r="H44" s="71">
+      <c r="H44" s="56">
         <v>3.1</v>
       </c>
-      <c r="J44" s="71">
+      <c r="J44" s="56">
         <f t="shared" si="0"/>
         <v>6.56</v>
       </c>
@@ -13282,13 +13256,13 @@
       <c r="F45" s="45">
         <v>27.6</v>
       </c>
-      <c r="G45" s="71">
+      <c r="G45" s="56">
         <v>37.4</v>
       </c>
-      <c r="H45" s="71">
+      <c r="H45" s="56">
         <v>39.4</v>
       </c>
-      <c r="J45" s="71">
+      <c r="J45" s="56">
         <f t="shared" si="0"/>
         <v>30.720000000000006</v>
       </c>
@@ -13312,13 +13286,13 @@
       <c r="F46" s="45">
         <v>10.6</v>
       </c>
-      <c r="G46" s="71">
+      <c r="G46" s="56">
         <v>47.7</v>
       </c>
-      <c r="H46" s="71">
+      <c r="H46" s="56">
         <v>24.4</v>
       </c>
-      <c r="J46" s="71">
+      <c r="J46" s="56">
         <f t="shared" si="0"/>
         <v>20.76</v>
       </c>
@@ -13342,13 +13316,13 @@
       <c r="F47" s="45">
         <v>48.6</v>
       </c>
-      <c r="G47" s="71">
+      <c r="G47" s="56">
         <v>72.099999999999994</v>
       </c>
-      <c r="H47" s="71">
+      <c r="H47" s="56">
         <v>51</v>
       </c>
-      <c r="J47" s="71">
+      <c r="J47" s="56">
         <f t="shared" si="0"/>
         <v>52.92</v>
       </c>
@@ -13372,13 +13346,13 @@
       <c r="F48" s="45">
         <v>12.9</v>
       </c>
-      <c r="G48" s="71">
+      <c r="G48" s="56">
         <v>20.6</v>
       </c>
-      <c r="H48" s="71">
+      <c r="H48" s="56">
         <v>23.2</v>
       </c>
-      <c r="J48" s="71">
+      <c r="J48" s="56">
         <f t="shared" si="0"/>
         <v>19.580000000000002</v>
       </c>
@@ -13402,13 +13376,13 @@
       <c r="F49" s="45">
         <v>21.1</v>
       </c>
-      <c r="G49" s="71">
+      <c r="G49" s="56">
         <v>23.5</v>
       </c>
-      <c r="H49" s="71">
+      <c r="H49" s="56">
         <v>23.8</v>
       </c>
-      <c r="J49" s="71">
+      <c r="J49" s="56">
         <f t="shared" si="0"/>
         <v>22.12</v>
       </c>
@@ -13432,13 +13406,13 @@
       <c r="F50" s="45">
         <v>4.5</v>
       </c>
-      <c r="G50" s="71">
-        <v>0</v>
-      </c>
-      <c r="H50" s="71">
-        <v>0</v>
-      </c>
-      <c r="J50" s="71">
+      <c r="G50" s="56">
+        <v>0</v>
+      </c>
+      <c r="H50" s="56">
+        <v>0</v>
+      </c>
+      <c r="J50" s="56">
         <f t="shared" si="0"/>
         <v>3.54</v>
       </c>
@@ -13456,31 +13430,31 @@
       <c r="F51" s="45">
         <v>0</v>
       </c>
-      <c r="G51" s="71">
+      <c r="G51" s="56">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H51" s="71">
+      <c r="H51" s="56">
         <v>19.8</v>
       </c>
-      <c r="J51" s="71">
+      <c r="J51" s="56">
         <f t="shared" si="0"/>
         <v>9.3666666666666671</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.3">
-      <c r="A52" s="71">
+    <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="56">
         <v>50488</v>
       </c>
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="56" t="s">
         <v>191</v>
       </c>
-      <c r="C52" s="72" t="s">
+      <c r="C52" s="57" t="s">
         <v>236</v>
       </c>
-      <c r="H52" s="71">
+      <c r="H52" s="56">
         <v>3.9</v>
       </c>
-      <c r="J52" s="71">
+      <c r="J52" s="56">
         <f t="shared" si="0"/>
         <v>3.9</v>
       </c>

</xml_diff>